<commit_message>
update fixture with new set of applications
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.17.mip_balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.17.mip_balsamic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19AE2D9-1A5F-9542-A6CB-8CB86C59766E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40B314E-61BD-C34D-B6F2-2E005F2FE970}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="3820" windowWidth="40440" windowHeight="24580" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3560" yWindow="1180" windowWidth="33060" windowHeight="25340" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Drop down lists" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="description" localSheetId="2">'Drop down lists'!$C$28</definedName>
+    <definedName name="description" localSheetId="2">'Drop down lists'!$C$29</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="530">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -1632,15 +1632,6 @@
     <t>WGLLIFC030</t>
   </si>
   <si>
-    <t>EXOTTTR125</t>
-  </si>
-  <si>
-    <t>EXTTTTR025</t>
-  </si>
-  <si>
-    <t>EXTTTTR050</t>
-  </si>
-  <si>
     <t>EXLTTTR020</t>
   </si>
   <si>
@@ -1711,9 +1702,6 @@
   </si>
   <si>
     <t>Updated Application tags</t>
-  </si>
-  <si>
-    <t>Nuclease free water</t>
   </si>
   <si>
     <t>Other (specify in "Comments")</t>
@@ -1776,181 +1764,319 @@
     </r>
   </si>
   <si>
+    <t>UDF/Capture Library version</t>
+  </si>
+  <si>
+    <t>UDF/Sample Buffer</t>
+  </si>
+  <si>
+    <t>10 mM Tris-HCl</t>
+  </si>
+  <si>
+    <t>Nuclease-free water</t>
+  </si>
+  <si>
+    <t>EB-buffer</t>
+  </si>
+  <si>
+    <t>EXOTTTR120</t>
+  </si>
+  <si>
+    <t>EXOTTTR140</t>
+  </si>
+  <si>
+    <t>EXTTTTR020</t>
+  </si>
+  <si>
+    <t>EXTTTTR040</t>
+  </si>
+  <si>
+    <t>whole-genome-1</t>
+  </si>
+  <si>
+    <t>whole-genome-2</t>
+  </si>
+  <si>
+    <t>whole-genome-3</t>
+  </si>
+  <si>
+    <t>whole-genome-4</t>
+  </si>
+  <si>
+    <t>whole-genome-5</t>
+  </si>
+  <si>
+    <t>whole-genome-6</t>
+  </si>
+  <si>
+    <t>whole-genome-7</t>
+  </si>
+  <si>
+    <t>whole-exome-1</t>
+  </si>
+  <si>
+    <t>whole-exome-2</t>
+  </si>
+  <si>
+    <t>whole-exome-3</t>
+  </si>
+  <si>
+    <t>whole-exome-4</t>
+  </si>
+  <si>
+    <t>whole-exome-5</t>
+  </si>
+  <si>
+    <t>whole-exome-6</t>
+  </si>
+  <si>
+    <t>whole-exome-7</t>
+  </si>
+  <si>
+    <t>whole-exome-8</t>
+  </si>
+  <si>
+    <t>whole-exome-9</t>
+  </si>
+  <si>
+    <t>whole-exome-10</t>
+  </si>
+  <si>
+    <t>whole-exome-11</t>
+  </si>
+  <si>
+    <t>whole-exome-12</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-1</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-2</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-3</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-4</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-5</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-6</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-7</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-8</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-9</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-10</t>
+  </si>
+  <si>
+    <t>rna-1</t>
+  </si>
+  <si>
+    <t>rna-2</t>
+  </si>
+  <si>
+    <t>rna-3</t>
+  </si>
+  <si>
+    <t>rna-4</t>
+  </si>
+  <si>
+    <t>rna-5</t>
+  </si>
+  <si>
+    <t>gene-list-test-1</t>
+  </si>
+  <si>
+    <t>gene-list-test-2</t>
+  </si>
+  <si>
+    <t>gene-list-test-3</t>
+  </si>
+  <si>
+    <t>gene-list-test-4</t>
+  </si>
+  <si>
+    <t>gene-list-test-5</t>
+  </si>
+  <si>
+    <t>gene-list-test-6</t>
+  </si>
+  <si>
+    <t>gene-list-test-7</t>
+  </si>
+  <si>
+    <t>gene-list-test-8</t>
+  </si>
+  <si>
+    <t>gene-list-test-9</t>
+  </si>
+  <si>
+    <t>plate</t>
+  </si>
+  <si>
+    <t>LymphoMATIC</t>
+  </si>
+  <si>
+    <t>GIcfDNA</t>
+  </si>
+  <si>
+    <t>GMCKsolid</t>
+  </si>
+  <si>
+    <t>GMSmyeloid</t>
+  </si>
+  <si>
+    <t>other (specify in comment field)</t>
+  </si>
+  <si>
+    <t>Nuclease free water</t>
+  </si>
+  <si>
     <t>Tris-HCl (pH 8-8.5)</t>
   </si>
   <si>
-    <t>UDF/Capture Library version</t>
-  </si>
-  <si>
-    <t>whole-genome-1</t>
-  </si>
-  <si>
-    <t>whole-genome</t>
-  </si>
-  <si>
-    <t>whole-genome-2</t>
-  </si>
-  <si>
-    <t>whole-genome-3</t>
-  </si>
-  <si>
-    <t>whole-genome-4</t>
-  </si>
-  <si>
-    <t>whole-genome-5</t>
-  </si>
-  <si>
-    <t>whole-genome-6</t>
-  </si>
-  <si>
-    <t>whole-genome-7</t>
-  </si>
-  <si>
-    <t>whole-exome-1</t>
-  </si>
-  <si>
-    <t>whole-exome</t>
-  </si>
-  <si>
-    <t>whole-exome-2</t>
-  </si>
-  <si>
-    <t>whole-exome-3</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-1</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-2</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-3</t>
-  </si>
-  <si>
-    <t>rna-1</t>
-  </si>
-  <si>
-    <t>rna</t>
-  </si>
-  <si>
-    <t>rna-2</t>
-  </si>
-  <si>
-    <t>gene-list-test-1</t>
-  </si>
-  <si>
-    <t>gene-list-test</t>
-  </si>
-  <si>
-    <t>gene-list-test-2</t>
-  </si>
-  <si>
-    <t>gene-list-test-3</t>
-  </si>
-  <si>
-    <t>gene-list-test-4</t>
-  </si>
-  <si>
-    <t>gene-list-test-5</t>
-  </si>
-  <si>
-    <t>gene-list-test-6</t>
-  </si>
-  <si>
-    <t>gene-list-test-7</t>
-  </si>
-  <si>
-    <t>gene-list-test-8</t>
-  </si>
-  <si>
-    <t>gene-list-test-9</t>
-  </si>
-  <si>
-    <t>plate</t>
-  </si>
-  <si>
-    <t>LymphoMATIC</t>
-  </si>
-  <si>
-    <t>GIcfDNA</t>
-  </si>
-  <si>
-    <t>GMCKsolid</t>
-  </si>
-  <si>
-    <t>GMSmyeloid</t>
-  </si>
-  <si>
-    <t>other (specify in comment field)</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
     <t>comment</t>
   </si>
   <si>
-    <t>whole-exome-4</t>
-  </si>
-  <si>
-    <t>whole-exome-5</t>
-  </si>
-  <si>
-    <t>whole-exome-6</t>
-  </si>
-  <si>
-    <t>whole-exome-7</t>
-  </si>
-  <si>
-    <t>whole-exome-8</t>
-  </si>
-  <si>
-    <t>whole-exome-9</t>
-  </si>
-  <si>
-    <t>whole-exome-10</t>
-  </si>
-  <si>
-    <t>whole-exome-11</t>
-  </si>
-  <si>
-    <t>whole-exome-12</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-4</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-5</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-6</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-7</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-8</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-9</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-10</t>
-  </si>
-  <si>
-    <t>rna-3</t>
-  </si>
-  <si>
-    <t>rna-4</t>
-  </si>
-  <si>
-    <t>rna-5</t>
-  </si>
-  <si>
-    <t>UDF/Sample Buffer</t>
+    <t>case-1</t>
+  </si>
+  <si>
+    <t>case-2</t>
+  </si>
+  <si>
+    <t>case-3</t>
+  </si>
+  <si>
+    <t>case-4</t>
+  </si>
+  <si>
+    <t>case-5</t>
+  </si>
+  <si>
+    <t>case-6</t>
+  </si>
+  <si>
+    <t>case-7</t>
+  </si>
+  <si>
+    <t>case-8</t>
+  </si>
+  <si>
+    <t>case-9</t>
+  </si>
+  <si>
+    <t>case-10</t>
+  </si>
+  <si>
+    <t>case-11</t>
+  </si>
+  <si>
+    <t>case-12</t>
+  </si>
+  <si>
+    <t>case-13</t>
+  </si>
+  <si>
+    <t>case-14</t>
+  </si>
+  <si>
+    <t>case-15</t>
+  </si>
+  <si>
+    <t>case-16</t>
+  </si>
+  <si>
+    <t>case-17</t>
+  </si>
+  <si>
+    <t>case-18</t>
+  </si>
+  <si>
+    <t>case-19</t>
+  </si>
+  <si>
+    <t>case-20</t>
+  </si>
+  <si>
+    <t>case-21</t>
+  </si>
+  <si>
+    <t>case-22</t>
+  </si>
+  <si>
+    <t>case-23</t>
+  </si>
+  <si>
+    <t>case-24</t>
+  </si>
+  <si>
+    <t>case-25</t>
+  </si>
+  <si>
+    <t>case-26</t>
+  </si>
+  <si>
+    <t>case-27</t>
+  </si>
+  <si>
+    <t>case-28</t>
+  </si>
+  <si>
+    <t>case-29</t>
+  </si>
+  <si>
+    <t>case-30</t>
+  </si>
+  <si>
+    <t>case-31</t>
+  </si>
+  <si>
+    <t>case-32</t>
+  </si>
+  <si>
+    <t>case-33</t>
+  </si>
+  <si>
+    <t>case-34</t>
+  </si>
+  <si>
+    <t>case-35</t>
+  </si>
+  <si>
+    <t>case-36</t>
+  </si>
+  <si>
+    <t>case-37</t>
+  </si>
+  <si>
+    <t>case-38</t>
+  </si>
+  <si>
+    <t>case-39</t>
+  </si>
+  <si>
+    <t>case-40</t>
+  </si>
+  <si>
+    <t>case-41</t>
+  </si>
+  <si>
+    <t>case-42</t>
+  </si>
+  <si>
+    <t>case-43</t>
   </si>
 </sst>
 </file>
@@ -2902,7 +3028,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="211">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3447,11 +3573,7 @@
     <xf numFmtId="0" fontId="32" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="47" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3492,6 +3614,13 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="47" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="334">
@@ -3923,8 +4052,8 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2310553</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>217594</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>44874</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4315,7 +4444,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4359,7 +4488,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4383,8 +4512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4413,7 +4542,7 @@
       <c r="D2" s="9"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" hidden="1">
+    <row r="3" spans="1:5" ht="13" hidden="1" customHeight="1">
       <c r="A3" s="12"/>
       <c r="B3" s="12" t="s">
         <v>23</v>
@@ -4425,7 +4554,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="170">
-        <v>43594</v>
+        <v>43605</v>
       </c>
     </row>
     <row r="4" spans="1:5" hidden="1">
@@ -4444,9 +4573,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14" hidden="1" customHeight="1"/>
-    <row r="6" spans="1:5" ht="1" hidden="1" customHeight="1"/>
-    <row r="7" spans="1:5" ht="1" hidden="1" customHeight="1"/>
-    <row r="8" spans="1:5" hidden="1"/>
+    <row r="6" spans="1:5" ht="14" hidden="1" customHeight="1"/>
+    <row r="8" spans="1:5" ht="12" customHeight="1"/>
+    <row r="9" spans="1:5" ht="14" customHeight="1"/>
     <row r="14" spans="1:5" ht="19">
       <c r="A14" s="40" t="s">
         <v>248</v>
@@ -4459,7 +4588,7 @@
     </row>
     <row r="16" spans="1:5" ht="14">
       <c r="A16" s="15" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="14">
@@ -4469,17 +4598,17 @@
     </row>
     <row r="18" spans="1:1" ht="14">
       <c r="A18" s="15" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="14">
       <c r="A19" s="15" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="14">
       <c r="A20" s="15" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="16">
@@ -4565,7 +4694,7 @@
     </row>
     <row r="39" spans="1:5" ht="28">
       <c r="A39" s="34" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C39" s="15"/>
       <c r="E39" s="15"/>
@@ -4613,7 +4742,7 @@
     </row>
     <row r="50" spans="1:1" ht="28">
       <c r="A50" s="34" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="51" spans="1:1">
@@ -4626,7 +4755,7 @@
     </row>
     <row r="53" spans="1:1" ht="42">
       <c r="A53" s="176" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="54" spans="1:1">
@@ -4718,7 +4847,7 @@
       <c r="A83" s="15"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9RBRmiHQiWKUjnTrxAAeo604h6ddJA24/1hpreXw4rnwxS1h/CtP1B7pJZMbY5om9yLYzr2p8pO8uQfbpgX3VQ==" saltValue="FYhtGQ/zzJzcwQcnkKcBuA==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="4hxgLibnT+qvSFmfmjUMHWExefFntKM8u3f5i5xQxyRSRuhWb0bB907+FMarbA98InnIUuJdSJ1l39nY4mbIbg==" saltValue="MY1gDBRgAtdf2sAb/ggfWQ==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
     <hyperlink ref="A14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
@@ -4740,8 +4869,8 @@
   </sheetPr>
   <dimension ref="A1:AE428"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="AD16" sqref="AD16:AE16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -5035,53 +5164,53 @@
       <c r="AE8" s="96"/>
     </row>
     <row r="9" spans="1:31" s="102" customFormat="1" ht="22" customHeight="1" outlineLevel="1">
-      <c r="A9" s="199" t="s">
+      <c r="A9" s="198" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="200"/>
-      <c r="C9" s="200"/>
-      <c r="D9" s="200"/>
-      <c r="E9" s="200"/>
-      <c r="F9" s="200"/>
-      <c r="G9" s="200"/>
-      <c r="H9" s="200"/>
-      <c r="I9" s="200"/>
-      <c r="J9" s="200"/>
-      <c r="K9" s="201"/>
+      <c r="B9" s="199"/>
+      <c r="C9" s="199"/>
+      <c r="D9" s="199"/>
+      <c r="E9" s="199"/>
+      <c r="F9" s="199"/>
+      <c r="G9" s="199"/>
+      <c r="H9" s="199"/>
+      <c r="I9" s="199"/>
+      <c r="J9" s="199"/>
+      <c r="K9" s="200"/>
       <c r="L9" s="98"/>
-      <c r="M9" s="202" t="s">
+      <c r="M9" s="201" t="s">
         <v>104</v>
       </c>
-      <c r="N9" s="203"/>
+      <c r="N9" s="202"/>
       <c r="O9" s="99"/>
-      <c r="P9" s="205" t="s">
+      <c r="P9" s="204" t="s">
         <v>349</v>
       </c>
-      <c r="Q9" s="206"/>
-      <c r="R9" s="206"/>
-      <c r="S9" s="207"/>
+      <c r="Q9" s="205"/>
+      <c r="R9" s="205"/>
+      <c r="S9" s="206"/>
       <c r="T9" s="100"/>
       <c r="U9" s="183" t="s">
         <v>383</v>
       </c>
       <c r="V9" s="101"/>
-      <c r="W9" s="198" t="s">
+      <c r="W9" s="197" t="s">
         <v>384</v>
       </c>
-      <c r="X9" s="198"/>
+      <c r="X9" s="197"/>
       <c r="Y9" s="101"/>
-      <c r="Z9" s="208" t="s">
+      <c r="Z9" s="207" t="s">
         <v>350</v>
       </c>
-      <c r="AA9" s="209"/>
-      <c r="AB9" s="210"/>
+      <c r="AA9" s="208"/>
+      <c r="AB9" s="209"/>
       <c r="AC9" s="100"/>
-      <c r="AD9" s="204" t="s">
+      <c r="AD9" s="203" t="s">
         <v>205</v>
       </c>
-      <c r="AE9" s="204"/>
-    </row>
-    <row r="10" spans="1:31" s="102" customFormat="1" ht="13" customHeight="1">
+      <c r="AE9" s="203"/>
+    </row>
+    <row r="10" spans="1:31" s="102" customFormat="1" ht="13" hidden="1" customHeight="1">
       <c r="A10" s="103" t="s">
         <v>0</v>
       </c>
@@ -5116,7 +5245,7 @@
       <c r="AD10" s="104"/>
       <c r="AE10" s="104"/>
     </row>
-    <row r="11" spans="1:31" s="118" customFormat="1" ht="41" customHeight="1">
+    <row r="11" spans="1:31" s="118" customFormat="1" ht="41" hidden="1" customHeight="1">
       <c r="A11" s="106" t="s">
         <v>1</v>
       </c>
@@ -5172,11 +5301,11 @@
       </c>
       <c r="T11" s="114"/>
       <c r="U11" s="194" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="V11" s="179"/>
       <c r="W11" s="195" t="s">
-        <v>487</v>
+        <v>426</v>
       </c>
       <c r="X11" s="115" t="s">
         <v>278</v>
@@ -5199,7 +5328,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="12" spans="1:31" s="126" customFormat="1" ht="19" customHeight="1">
+    <row r="12" spans="1:31" s="126" customFormat="1" ht="19" hidden="1" customHeight="1">
       <c r="A12" s="103" t="s">
         <v>5</v>
       </c>
@@ -5294,7 +5423,7 @@
       </c>
       <c r="V13" s="181"/>
       <c r="W13" s="140" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="X13" s="140" t="s">
         <v>296</v>
@@ -5317,7 +5446,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:31" s="126" customFormat="1" ht="13" customHeight="1">
+    <row r="14" spans="1:31" s="126" customFormat="1" ht="13" hidden="1" customHeight="1">
       <c r="A14" s="145" t="s">
         <v>6</v>
       </c>
@@ -5354,7 +5483,7 @@
     </row>
     <row r="15" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A15" s="55" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B15" s="53" t="s">
         <v>37</v>
@@ -5366,7 +5495,7 @@
         <v>285</v>
       </c>
       <c r="E15" s="55" t="s">
-        <v>432</v>
+        <v>487</v>
       </c>
       <c r="F15" s="54" t="s">
         <v>15</v>
@@ -5388,7 +5517,7 @@
       </c>
       <c r="L15" s="149"/>
       <c r="M15" s="58" t="s">
-        <v>460</v>
+        <v>477</v>
       </c>
       <c r="N15" s="57" t="s">
         <v>27</v>
@@ -5401,18 +5530,18 @@
         <v>300</v>
       </c>
       <c r="R15" s="55" t="s">
-        <v>433</v>
-      </c>
-      <c r="S15" s="197" t="s">
-        <v>434</v>
+        <v>435</v>
+      </c>
+      <c r="S15" s="211" t="s">
+        <v>436</v>
       </c>
       <c r="T15" s="150"/>
       <c r="U15" s="21" t="s">
-        <v>461</v>
+        <v>478</v>
       </c>
       <c r="V15" s="180"/>
       <c r="W15" s="61" t="s">
-        <v>422</v>
+        <v>483</v>
       </c>
       <c r="X15" s="21">
         <v>5</v>
@@ -5429,15 +5558,15 @@
       </c>
       <c r="AC15" s="152"/>
       <c r="AD15" s="58" t="s">
-        <v>466</v>
+        <v>485</v>
       </c>
       <c r="AE15" s="58" t="s">
-        <v>467</v>
+        <v>486</v>
       </c>
     </row>
     <row r="16" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A16" s="55" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B16" s="53" t="s">
         <v>37</v>
@@ -5449,7 +5578,7 @@
         <v>290</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>432</v>
+        <v>488</v>
       </c>
       <c r="F16" s="54" t="s">
         <v>16</v>
@@ -5483,7 +5612,7 @@
       <c r="S16" s="60"/>
       <c r="T16" s="150"/>
       <c r="U16" s="33" t="s">
-        <v>462</v>
+        <v>479</v>
       </c>
       <c r="V16" s="180"/>
       <c r="W16" s="61"/>
@@ -5502,7 +5631,7 @@
     </row>
     <row r="17" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A17" s="55" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B17" s="53" t="s">
         <v>37</v>
@@ -5514,7 +5643,7 @@
         <v>286</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>432</v>
+        <v>489</v>
       </c>
       <c r="F17" s="54" t="s">
         <v>15</v>
@@ -5548,7 +5677,7 @@
       <c r="S17" s="60"/>
       <c r="T17" s="150"/>
       <c r="U17" s="21" t="s">
-        <v>463</v>
+        <v>480</v>
       </c>
       <c r="V17" s="180"/>
       <c r="W17" s="61"/>
@@ -5565,7 +5694,7 @@
     </row>
     <row r="18" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A18" s="55" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B18" s="53" t="s">
         <v>37</v>
@@ -5577,7 +5706,7 @@
         <v>287</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>432</v>
+        <v>490</v>
       </c>
       <c r="F18" s="54" t="s">
         <v>77</v>
@@ -5611,7 +5740,7 @@
       <c r="S18" s="60"/>
       <c r="T18" s="150"/>
       <c r="U18" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V18" s="180"/>
       <c r="W18" s="61"/>
@@ -5628,7 +5757,7 @@
     </row>
     <row r="19" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A19" s="55" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B19" s="53" t="s">
         <v>37</v>
@@ -5640,7 +5769,7 @@
         <v>288</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>432</v>
+        <v>491</v>
       </c>
       <c r="F19" s="54" t="s">
         <v>77</v>
@@ -5674,7 +5803,7 @@
       <c r="S19" s="60"/>
       <c r="T19" s="150"/>
       <c r="U19" s="21" t="s">
-        <v>465</v>
+        <v>482</v>
       </c>
       <c r="V19" s="180"/>
       <c r="W19" s="61"/>
@@ -5691,7 +5820,7 @@
     </row>
     <row r="20" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A20" s="55" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B20" s="53" t="s">
         <v>37</v>
@@ -5703,7 +5832,7 @@
         <v>289</v>
       </c>
       <c r="E20" s="55" t="s">
-        <v>432</v>
+        <v>492</v>
       </c>
       <c r="F20" s="54" t="s">
         <v>77</v>
@@ -5737,7 +5866,7 @@
       <c r="S20" s="60"/>
       <c r="T20" s="150"/>
       <c r="U20" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V20" s="180"/>
       <c r="W20" s="61"/>
@@ -5754,7 +5883,7 @@
     </row>
     <row r="21" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A21" s="55" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B21" s="53" t="s">
         <v>37</v>
@@ -5766,7 +5895,7 @@
         <v>394</v>
       </c>
       <c r="E21" s="55" t="s">
-        <v>432</v>
+        <v>493</v>
       </c>
       <c r="F21" s="54" t="s">
         <v>77</v>
@@ -5800,7 +5929,7 @@
       <c r="S21" s="60"/>
       <c r="T21" s="150"/>
       <c r="U21" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V21" s="180"/>
       <c r="W21" s="61"/>
@@ -5817,7 +5946,7 @@
     </row>
     <row r="22" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A22" s="55" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B22" s="53" t="s">
         <v>37</v>
@@ -5829,7 +5958,7 @@
         <v>389</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>440</v>
+        <v>494</v>
       </c>
       <c r="F22" s="54" t="s">
         <v>77</v>
@@ -5863,7 +5992,7 @@
       <c r="S22" s="60"/>
       <c r="T22" s="150"/>
       <c r="U22" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V22" s="180"/>
       <c r="W22" s="61"/>
@@ -5880,7 +6009,7 @@
     </row>
     <row r="23" spans="1:31" ht="25" customHeight="1">
       <c r="A23" s="55" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B23" s="53" t="s">
         <v>37</v>
@@ -5892,7 +6021,7 @@
         <v>390</v>
       </c>
       <c r="E23" s="55" t="s">
-        <v>440</v>
+        <v>495</v>
       </c>
       <c r="F23" s="54" t="s">
         <v>77</v>
@@ -5926,7 +6055,7 @@
       <c r="S23" s="60"/>
       <c r="T23" s="150"/>
       <c r="U23" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V23" s="180"/>
       <c r="W23" s="61"/>
@@ -5943,7 +6072,7 @@
     </row>
     <row r="24" spans="1:31" ht="25" customHeight="1">
       <c r="A24" s="55" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B24" s="53" t="s">
         <v>37</v>
@@ -5955,7 +6084,7 @@
         <v>391</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>440</v>
+        <v>496</v>
       </c>
       <c r="F24" s="54" t="s">
         <v>77</v>
@@ -5963,7 +6092,7 @@
       <c r="G24" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H24" s="196" t="s">
+      <c r="H24" s="210" t="s">
         <v>356</v>
       </c>
       <c r="I24" s="20" t="s">
@@ -5989,7 +6118,7 @@
       <c r="S24" s="60"/>
       <c r="T24" s="150"/>
       <c r="U24" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V24" s="180"/>
       <c r="W24" s="61"/>
@@ -6006,7 +6135,7 @@
     </row>
     <row r="25" spans="1:31" ht="25" customHeight="1">
       <c r="A25" s="55" t="s">
-        <v>468</v>
+        <v>444</v>
       </c>
       <c r="B25" s="53" t="s">
         <v>37</v>
@@ -6018,7 +6147,7 @@
         <v>392</v>
       </c>
       <c r="E25" s="55" t="s">
-        <v>440</v>
+        <v>497</v>
       </c>
       <c r="F25" s="54" t="s">
         <v>77</v>
@@ -6026,7 +6155,7 @@
       <c r="G25" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H25" s="196" t="s">
+      <c r="H25" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I25" s="20" t="s">
@@ -6052,11 +6181,11 @@
       <c r="S25" s="60"/>
       <c r="T25" s="150"/>
       <c r="U25" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V25" s="180"/>
       <c r="W25" s="61" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="X25" s="21">
         <v>55</v>
@@ -6071,7 +6200,7 @@
     </row>
     <row r="26" spans="1:31" ht="25" customHeight="1">
       <c r="A26" s="55" t="s">
-        <v>469</v>
+        <v>445</v>
       </c>
       <c r="B26" s="53" t="s">
         <v>37</v>
@@ -6083,7 +6212,7 @@
         <v>381</v>
       </c>
       <c r="E26" s="55" t="s">
-        <v>440</v>
+        <v>498</v>
       </c>
       <c r="F26" s="54" t="s">
         <v>77</v>
@@ -6117,11 +6246,11 @@
       <c r="S26" s="60"/>
       <c r="T26" s="150"/>
       <c r="U26" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V26" s="180"/>
       <c r="W26" s="61" t="s">
-        <v>429</v>
+        <v>484</v>
       </c>
       <c r="X26" s="21">
         <v>60</v>
@@ -6136,7 +6265,7 @@
     </row>
     <row r="27" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A27" s="55" t="s">
-        <v>470</v>
+        <v>446</v>
       </c>
       <c r="B27" s="53" t="s">
         <v>37</v>
@@ -6145,10 +6274,10 @@
         <v>354</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="E27" s="55" t="s">
-        <v>440</v>
+        <v>499</v>
       </c>
       <c r="F27" s="54" t="s">
         <v>77</v>
@@ -6156,7 +6285,7 @@
       <c r="G27" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H27" s="196" t="s">
+      <c r="H27" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I27" s="20" t="s">
@@ -6182,11 +6311,11 @@
       <c r="S27" s="60"/>
       <c r="T27" s="150"/>
       <c r="U27" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V27" s="180"/>
       <c r="W27" s="61" t="s">
-        <v>422</v>
+        <v>483</v>
       </c>
       <c r="X27" s="21">
         <v>65</v>
@@ -6201,7 +6330,7 @@
     </row>
     <row r="28" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A28" s="55" t="s">
-        <v>471</v>
+        <v>447</v>
       </c>
       <c r="B28" s="53" t="s">
         <v>37</v>
@@ -6210,10 +6339,10 @@
         <v>354</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>396</v>
+        <v>431</v>
       </c>
       <c r="E28" s="55" t="s">
-        <v>440</v>
+        <v>500</v>
       </c>
       <c r="F28" s="54" t="s">
         <v>77</v>
@@ -6221,7 +6350,7 @@
       <c r="G28" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H28" s="196" t="s">
+      <c r="H28" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I28" s="20" t="s">
@@ -6247,11 +6376,11 @@
       <c r="S28" s="60"/>
       <c r="T28" s="150"/>
       <c r="U28" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V28" s="180"/>
       <c r="W28" s="61" t="s">
-        <v>422</v>
+        <v>483</v>
       </c>
       <c r="X28" s="21">
         <v>70</v>
@@ -6266,7 +6395,7 @@
     </row>
     <row r="29" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A29" s="55" t="s">
-        <v>472</v>
+        <v>448</v>
       </c>
       <c r="B29" s="53" t="s">
         <v>37</v>
@@ -6275,10 +6404,10 @@
         <v>354</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>397</v>
+        <v>432</v>
       </c>
       <c r="E29" s="55" t="s">
-        <v>440</v>
+        <v>501</v>
       </c>
       <c r="F29" s="54" t="s">
         <v>77</v>
@@ -6286,7 +6415,7 @@
       <c r="G29" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H29" s="196" t="s">
+      <c r="H29" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I29" s="20" t="s">
@@ -6312,11 +6441,11 @@
       <c r="S29" s="60"/>
       <c r="T29" s="150"/>
       <c r="U29" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V29" s="180"/>
       <c r="W29" s="61" t="s">
-        <v>422</v>
+        <v>483</v>
       </c>
       <c r="X29" s="21">
         <v>75</v>
@@ -6331,7 +6460,7 @@
     </row>
     <row r="30" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A30" s="55" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
       <c r="B30" s="53" t="s">
         <v>37</v>
@@ -6340,10 +6469,10 @@
         <v>354</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>398</v>
+        <v>433</v>
       </c>
       <c r="E30" s="55" t="s">
-        <v>440</v>
+        <v>502</v>
       </c>
       <c r="F30" s="54" t="s">
         <v>77</v>
@@ -6351,7 +6480,7 @@
       <c r="G30" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H30" s="196" t="s">
+      <c r="H30" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I30" s="20" t="s">
@@ -6377,11 +6506,11 @@
       <c r="S30" s="60"/>
       <c r="T30" s="150"/>
       <c r="U30" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V30" s="180"/>
       <c r="W30" s="61" t="s">
-        <v>422</v>
+        <v>483</v>
       </c>
       <c r="X30" s="21">
         <v>80</v>
@@ -6396,7 +6525,7 @@
     </row>
     <row r="31" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A31" s="55" t="s">
-        <v>474</v>
+        <v>450</v>
       </c>
       <c r="B31" s="53" t="s">
         <v>37</v>
@@ -6405,10 +6534,10 @@
         <v>354</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="E31" s="55" t="s">
-        <v>440</v>
+        <v>503</v>
       </c>
       <c r="F31" s="54" t="s">
         <v>77</v>
@@ -6416,7 +6545,7 @@
       <c r="G31" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H31" s="196" t="s">
+      <c r="H31" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I31" s="20" t="s">
@@ -6442,7 +6571,7 @@
       <c r="S31" s="60"/>
       <c r="T31" s="150"/>
       <c r="U31" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V31" s="180"/>
       <c r="W31" s="61"/>
@@ -6459,7 +6588,7 @@
     </row>
     <row r="32" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A32" s="55" t="s">
-        <v>475</v>
+        <v>451</v>
       </c>
       <c r="B32" s="53" t="s">
         <v>37</v>
@@ -6468,10 +6597,10 @@
         <v>354</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="E32" s="55" t="s">
-        <v>440</v>
+        <v>504</v>
       </c>
       <c r="F32" s="54" t="s">
         <v>77</v>
@@ -6479,7 +6608,7 @@
       <c r="G32" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H32" s="196" t="s">
+      <c r="H32" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I32" s="20" t="s">
@@ -6505,7 +6634,7 @@
       <c r="S32" s="60"/>
       <c r="T32" s="150"/>
       <c r="U32" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V32" s="180"/>
       <c r="W32" s="61"/>
@@ -6522,7 +6651,7 @@
     </row>
     <row r="33" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A33" s="55" t="s">
-        <v>476</v>
+        <v>452</v>
       </c>
       <c r="B33" s="53" t="s">
         <v>37</v>
@@ -6531,10 +6660,10 @@
         <v>354</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="E33" s="55" t="s">
-        <v>440</v>
+        <v>505</v>
       </c>
       <c r="F33" s="54" t="s">
         <v>77</v>
@@ -6542,7 +6671,7 @@
       <c r="G33" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H33" s="196" t="s">
+      <c r="H33" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I33" s="20" t="s">
@@ -6568,7 +6697,7 @@
       <c r="S33" s="60"/>
       <c r="T33" s="150"/>
       <c r="U33" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V33" s="180"/>
       <c r="W33" s="61"/>
@@ -6585,7 +6714,7 @@
     </row>
     <row r="34" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A34" s="55" t="s">
-        <v>443</v>
+        <v>453</v>
       </c>
       <c r="B34" s="53" t="s">
         <v>37</v>
@@ -6594,10 +6723,10 @@
         <v>354</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="E34" s="55" t="s">
-        <v>444</v>
+        <v>506</v>
       </c>
       <c r="F34" s="54" t="s">
         <v>77</v>
@@ -6605,7 +6734,7 @@
       <c r="G34" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H34" s="196" t="s">
+      <c r="H34" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I34" s="20" t="s">
@@ -6631,7 +6760,7 @@
       <c r="S34" s="60"/>
       <c r="T34" s="150"/>
       <c r="U34" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V34" s="180"/>
       <c r="W34" s="61"/>
@@ -6648,7 +6777,7 @@
     </row>
     <row r="35" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A35" s="55" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
       <c r="B35" s="53" t="s">
         <v>37</v>
@@ -6657,10 +6786,10 @@
         <v>354</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="E35" s="55" t="s">
-        <v>444</v>
+        <v>507</v>
       </c>
       <c r="F35" s="54" t="s">
         <v>77</v>
@@ -6668,7 +6797,7 @@
       <c r="G35" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H35" s="196" t="s">
+      <c r="H35" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I35" s="20" t="s">
@@ -6694,7 +6823,7 @@
       <c r="S35" s="60"/>
       <c r="T35" s="150"/>
       <c r="U35" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V35" s="180"/>
       <c r="W35" s="61"/>
@@ -6711,7 +6840,7 @@
     </row>
     <row r="36" spans="1:31" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A36" s="55" t="s">
-        <v>446</v>
+        <v>455</v>
       </c>
       <c r="B36" s="53" t="s">
         <v>37</v>
@@ -6720,10 +6849,10 @@
         <v>354</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>249</v>
+        <v>404</v>
       </c>
       <c r="E36" s="55" t="s">
-        <v>444</v>
+        <v>508</v>
       </c>
       <c r="F36" s="54" t="s">
         <v>77</v>
@@ -6731,7 +6860,7 @@
       <c r="G36" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H36" s="196" t="s">
+      <c r="H36" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I36" s="20" t="s">
@@ -6757,7 +6886,7 @@
       <c r="S36" s="60"/>
       <c r="T36" s="150"/>
       <c r="U36" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V36" s="180"/>
       <c r="W36" s="61"/>
@@ -6774,7 +6903,7 @@
     </row>
     <row r="37" spans="1:31" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A37" s="55" t="s">
-        <v>477</v>
+        <v>456</v>
       </c>
       <c r="B37" s="53" t="s">
         <v>37</v>
@@ -6783,10 +6912,10 @@
         <v>354</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>408</v>
+        <v>249</v>
       </c>
       <c r="E37" s="55" t="s">
-        <v>444</v>
+        <v>509</v>
       </c>
       <c r="F37" s="54" t="s">
         <v>77</v>
@@ -6794,7 +6923,7 @@
       <c r="G37" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H37" s="196" t="s">
+      <c r="H37" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I37" s="20" t="s">
@@ -6820,7 +6949,7 @@
       <c r="S37" s="60"/>
       <c r="T37" s="150"/>
       <c r="U37" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V37" s="180"/>
       <c r="W37" s="61"/>
@@ -6837,7 +6966,7 @@
     </row>
     <row r="38" spans="1:31" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A38" s="55" t="s">
-        <v>478</v>
+        <v>457</v>
       </c>
       <c r="B38" s="53" t="s">
         <v>37</v>
@@ -6846,10 +6975,10 @@
         <v>354</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>364</v>
+        <v>405</v>
       </c>
       <c r="E38" s="55" t="s">
-        <v>444</v>
+        <v>510</v>
       </c>
       <c r="F38" s="54" t="s">
         <v>77</v>
@@ -6857,7 +6986,7 @@
       <c r="G38" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H38" s="196" t="s">
+      <c r="H38" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I38" s="20" t="s">
@@ -6883,7 +7012,7 @@
       <c r="S38" s="60"/>
       <c r="T38" s="150"/>
       <c r="U38" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V38" s="180"/>
       <c r="W38" s="61"/>
@@ -6900,7 +7029,7 @@
     </row>
     <row r="39" spans="1:31" ht="25" customHeight="1">
       <c r="A39" s="55" t="s">
-        <v>479</v>
+        <v>458</v>
       </c>
       <c r="B39" s="53" t="s">
         <v>37</v>
@@ -6909,10 +7038,10 @@
         <v>354</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>409</v>
+        <v>364</v>
       </c>
       <c r="E39" s="55" t="s">
-        <v>444</v>
+        <v>511</v>
       </c>
       <c r="F39" s="54" t="s">
         <v>77</v>
@@ -6920,7 +7049,7 @@
       <c r="G39" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H39" s="196" t="s">
+      <c r="H39" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I39" s="20" t="s">
@@ -6946,7 +7075,7 @@
       <c r="S39" s="60"/>
       <c r="T39" s="150"/>
       <c r="U39" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V39" s="180"/>
       <c r="W39" s="61"/>
@@ -6963,7 +7092,7 @@
     </row>
     <row r="40" spans="1:31" ht="25" customHeight="1">
       <c r="A40" s="55" t="s">
-        <v>480</v>
+        <v>459</v>
       </c>
       <c r="B40" s="53" t="s">
         <v>37</v>
@@ -6972,10 +7101,10 @@
         <v>354</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E40" s="55" t="s">
-        <v>444</v>
+        <v>512</v>
       </c>
       <c r="F40" s="54" t="s">
         <v>77</v>
@@ -6983,7 +7112,7 @@
       <c r="G40" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H40" s="196" t="s">
+      <c r="H40" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I40" s="20" t="s">
@@ -7009,7 +7138,7 @@
       <c r="S40" s="60"/>
       <c r="T40" s="150"/>
       <c r="U40" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V40" s="180"/>
       <c r="W40" s="61"/>
@@ -7026,7 +7155,7 @@
     </row>
     <row r="41" spans="1:31" ht="25" customHeight="1">
       <c r="A41" s="55" t="s">
-        <v>481</v>
+        <v>460</v>
       </c>
       <c r="B41" s="53" t="s">
         <v>37</v>
@@ -7035,10 +7164,10 @@
         <v>354</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="E41" s="55" t="s">
-        <v>444</v>
+        <v>513</v>
       </c>
       <c r="F41" s="54" t="s">
         <v>77</v>
@@ -7046,7 +7175,7 @@
       <c r="G41" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H41" s="196" t="s">
+      <c r="H41" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I41" s="20" t="s">
@@ -7072,7 +7201,7 @@
       <c r="S41" s="60"/>
       <c r="T41" s="150"/>
       <c r="U41" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V41" s="180"/>
       <c r="W41" s="61"/>
@@ -7089,7 +7218,7 @@
     </row>
     <row r="42" spans="1:31" ht="25" customHeight="1">
       <c r="A42" s="55" t="s">
-        <v>482</v>
+        <v>461</v>
       </c>
       <c r="B42" s="53" t="s">
         <v>37</v>
@@ -7098,10 +7227,10 @@
         <v>354</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="E42" s="55" t="s">
-        <v>444</v>
+        <v>514</v>
       </c>
       <c r="F42" s="54" t="s">
         <v>77</v>
@@ -7109,7 +7238,7 @@
       <c r="G42" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H42" s="196" t="s">
+      <c r="H42" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I42" s="20" t="s">
@@ -7135,7 +7264,7 @@
       <c r="S42" s="60"/>
       <c r="T42" s="150"/>
       <c r="U42" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V42" s="180"/>
       <c r="W42" s="61"/>
@@ -7152,7 +7281,7 @@
     </row>
     <row r="43" spans="1:31" ht="25" customHeight="1">
       <c r="A43" s="55" t="s">
-        <v>483</v>
+        <v>462</v>
       </c>
       <c r="B43" s="53" t="s">
         <v>37</v>
@@ -7161,10 +7290,10 @@
         <v>354</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="E43" s="55" t="s">
-        <v>444</v>
+        <v>515</v>
       </c>
       <c r="F43" s="54" t="s">
         <v>77</v>
@@ -7172,7 +7301,7 @@
       <c r="G43" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H43" s="196" t="s">
+      <c r="H43" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I43" s="20" t="s">
@@ -7198,7 +7327,7 @@
       <c r="S43" s="60"/>
       <c r="T43" s="150"/>
       <c r="U43" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V43" s="180"/>
       <c r="W43" s="61"/>
@@ -7215,7 +7344,7 @@
     </row>
     <row r="44" spans="1:31" ht="25" customHeight="1">
       <c r="A44" s="55" t="s">
-        <v>447</v>
+        <v>463</v>
       </c>
       <c r="B44" s="53" t="s">
         <v>37</v>
@@ -7224,10 +7353,10 @@
         <v>354</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="E44" s="55" t="s">
-        <v>448</v>
+        <v>516</v>
       </c>
       <c r="F44" s="54" t="s">
         <v>77</v>
@@ -7235,7 +7364,7 @@
       <c r="G44" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H44" s="196" t="s">
+      <c r="H44" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I44" s="20" t="s">
@@ -7261,7 +7390,7 @@
       <c r="S44" s="60"/>
       <c r="T44" s="150"/>
       <c r="U44" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V44" s="180"/>
       <c r="W44" s="61"/>
@@ -7278,7 +7407,7 @@
     </row>
     <row r="45" spans="1:31" ht="25" customHeight="1">
       <c r="A45" s="55" t="s">
-        <v>449</v>
+        <v>464</v>
       </c>
       <c r="B45" s="53" t="s">
         <v>37</v>
@@ -7287,10 +7416,10 @@
         <v>354</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="E45" s="55" t="s">
-        <v>448</v>
+        <v>517</v>
       </c>
       <c r="F45" s="54" t="s">
         <v>77</v>
@@ -7298,7 +7427,7 @@
       <c r="G45" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H45" s="196" t="s">
+      <c r="H45" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I45" s="20" t="s">
@@ -7324,7 +7453,7 @@
       <c r="S45" s="60"/>
       <c r="T45" s="150"/>
       <c r="U45" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V45" s="180"/>
       <c r="W45" s="61"/>
@@ -7341,7 +7470,7 @@
     </row>
     <row r="46" spans="1:31" ht="25" customHeight="1">
       <c r="A46" s="55" t="s">
-        <v>484</v>
+        <v>465</v>
       </c>
       <c r="B46" s="53" t="s">
         <v>37</v>
@@ -7350,10 +7479,10 @@
         <v>354</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="E46" s="55" t="s">
-        <v>448</v>
+        <v>518</v>
       </c>
       <c r="F46" s="54" t="s">
         <v>77</v>
@@ -7361,7 +7490,7 @@
       <c r="G46" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H46" s="196" t="s">
+      <c r="H46" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I46" s="20" t="s">
@@ -7387,7 +7516,7 @@
       <c r="S46" s="60"/>
       <c r="T46" s="150"/>
       <c r="U46" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V46" s="180"/>
       <c r="W46" s="61"/>
@@ -7404,7 +7533,7 @@
     </row>
     <row r="47" spans="1:31" ht="25" customHeight="1">
       <c r="A47" s="55" t="s">
-        <v>485</v>
+        <v>466</v>
       </c>
       <c r="B47" s="53" t="s">
         <v>37</v>
@@ -7413,10 +7542,10 @@
         <v>354</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="E47" s="55" t="s">
-        <v>448</v>
+        <v>519</v>
       </c>
       <c r="F47" s="54" t="s">
         <v>77</v>
@@ -7424,7 +7553,7 @@
       <c r="G47" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H47" s="196" t="s">
+      <c r="H47" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I47" s="20" t="s">
@@ -7450,7 +7579,7 @@
       <c r="S47" s="60"/>
       <c r="T47" s="150"/>
       <c r="U47" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V47" s="180"/>
       <c r="W47" s="61"/>
@@ -7467,7 +7596,7 @@
     </row>
     <row r="48" spans="1:31" ht="25" customHeight="1">
       <c r="A48" s="55" t="s">
-        <v>486</v>
+        <v>467</v>
       </c>
       <c r="B48" s="53" t="s">
         <v>37</v>
@@ -7476,10 +7605,10 @@
         <v>354</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E48" s="55" t="s">
-        <v>448</v>
+        <v>520</v>
       </c>
       <c r="F48" s="54" t="s">
         <v>77</v>
@@ -7487,7 +7616,7 @@
       <c r="G48" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H48" s="196" t="s">
+      <c r="H48" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I48" s="20" t="s">
@@ -7513,7 +7642,7 @@
       <c r="S48" s="60"/>
       <c r="T48" s="150"/>
       <c r="U48" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V48" s="180"/>
       <c r="W48" s="61"/>
@@ -7530,7 +7659,7 @@
     </row>
     <row r="49" spans="1:31" ht="25" customHeight="1">
       <c r="A49" s="39" t="s">
-        <v>450</v>
+        <v>468</v>
       </c>
       <c r="B49" s="53" t="s">
         <v>37</v>
@@ -7539,10 +7668,10 @@
         <v>354</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>285</v>
+        <v>415</v>
       </c>
       <c r="E49" s="55" t="s">
-        <v>451</v>
+        <v>521</v>
       </c>
       <c r="F49" s="54" t="s">
         <v>77</v>
@@ -7550,7 +7679,7 @@
       <c r="G49" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H49" s="196" t="s">
+      <c r="H49" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I49" s="20" t="s">
@@ -7576,7 +7705,7 @@
       <c r="S49" s="60"/>
       <c r="T49" s="150"/>
       <c r="U49" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V49" s="180"/>
       <c r="W49" s="61"/>
@@ -7593,7 +7722,7 @@
     </row>
     <row r="50" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A50" s="39" t="s">
-        <v>452</v>
+        <v>469</v>
       </c>
       <c r="B50" s="53" t="s">
         <v>37</v>
@@ -7605,7 +7734,7 @@
         <v>285</v>
       </c>
       <c r="E50" s="55" t="s">
-        <v>451</v>
+        <v>522</v>
       </c>
       <c r="F50" s="54" t="s">
         <v>77</v>
@@ -7613,7 +7742,7 @@
       <c r="G50" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H50" s="196" t="s">
+      <c r="H50" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I50" s="20" t="s">
@@ -7639,7 +7768,7 @@
       <c r="S50" s="60"/>
       <c r="T50" s="150"/>
       <c r="U50" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V50" s="180"/>
       <c r="W50" s="61"/>
@@ -7656,7 +7785,7 @@
     </row>
     <row r="51" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A51" s="39" t="s">
-        <v>453</v>
+        <v>470</v>
       </c>
       <c r="B51" s="53" t="s">
         <v>37</v>
@@ -7668,7 +7797,7 @@
         <v>285</v>
       </c>
       <c r="E51" s="55" t="s">
-        <v>451</v>
+        <v>523</v>
       </c>
       <c r="F51" s="54" t="s">
         <v>77</v>
@@ -7676,7 +7805,7 @@
       <c r="G51" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H51" s="196" t="s">
+      <c r="H51" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I51" s="20" t="s">
@@ -7702,7 +7831,7 @@
       <c r="S51" s="60"/>
       <c r="T51" s="150"/>
       <c r="U51" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V51" s="180"/>
       <c r="W51" s="61"/>
@@ -7719,7 +7848,7 @@
     </row>
     <row r="52" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A52" s="39" t="s">
-        <v>454</v>
+        <v>471</v>
       </c>
       <c r="B52" s="53" t="s">
         <v>37</v>
@@ -7731,7 +7860,7 @@
         <v>285</v>
       </c>
       <c r="E52" s="55" t="s">
-        <v>451</v>
+        <v>524</v>
       </c>
       <c r="F52" s="54" t="s">
         <v>77</v>
@@ -7739,7 +7868,7 @@
       <c r="G52" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H52" s="196" t="s">
+      <c r="H52" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I52" s="20" t="s">
@@ -7765,7 +7894,7 @@
       <c r="S52" s="60"/>
       <c r="T52" s="150"/>
       <c r="U52" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V52" s="180"/>
       <c r="W52" s="61"/>
@@ -7782,7 +7911,7 @@
     </row>
     <row r="53" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A53" s="39" t="s">
-        <v>455</v>
+        <v>472</v>
       </c>
       <c r="B53" s="53" t="s">
         <v>37</v>
@@ -7794,7 +7923,7 @@
         <v>285</v>
       </c>
       <c r="E53" s="55" t="s">
-        <v>451</v>
+        <v>525</v>
       </c>
       <c r="F53" s="54" t="s">
         <v>77</v>
@@ -7802,7 +7931,7 @@
       <c r="G53" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H53" s="196" t="s">
+      <c r="H53" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I53" s="20" t="s">
@@ -7828,7 +7957,7 @@
       <c r="S53" s="60"/>
       <c r="T53" s="150"/>
       <c r="U53" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V53" s="180"/>
       <c r="W53" s="61"/>
@@ -7845,7 +7974,7 @@
     </row>
     <row r="54" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A54" s="39" t="s">
-        <v>456</v>
+        <v>473</v>
       </c>
       <c r="B54" s="53" t="s">
         <v>37</v>
@@ -7857,7 +7986,7 @@
         <v>285</v>
       </c>
       <c r="E54" s="55" t="s">
-        <v>451</v>
+        <v>526</v>
       </c>
       <c r="F54" s="54" t="s">
         <v>77</v>
@@ -7865,7 +7994,7 @@
       <c r="G54" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H54" s="196" t="s">
+      <c r="H54" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I54" s="20" t="s">
@@ -7891,7 +8020,7 @@
       <c r="S54" s="60"/>
       <c r="T54" s="150"/>
       <c r="U54" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V54" s="180"/>
       <c r="W54" s="61"/>
@@ -7908,7 +8037,7 @@
     </row>
     <row r="55" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A55" s="39" t="s">
-        <v>457</v>
+        <v>474</v>
       </c>
       <c r="B55" s="53" t="s">
         <v>37</v>
@@ -7920,7 +8049,7 @@
         <v>285</v>
       </c>
       <c r="E55" s="55" t="s">
-        <v>451</v>
+        <v>527</v>
       </c>
       <c r="F55" s="54" t="s">
         <v>77</v>
@@ -7928,7 +8057,7 @@
       <c r="G55" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H55" s="196" t="s">
+      <c r="H55" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I55" s="20" t="s">
@@ -7954,7 +8083,7 @@
       <c r="S55" s="60"/>
       <c r="T55" s="150"/>
       <c r="U55" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V55" s="180"/>
       <c r="W55" s="61"/>
@@ -7971,7 +8100,7 @@
     </row>
     <row r="56" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A56" s="39" t="s">
-        <v>458</v>
+        <v>475</v>
       </c>
       <c r="B56" s="53" t="s">
         <v>37</v>
@@ -7983,7 +8112,7 @@
         <v>285</v>
       </c>
       <c r="E56" s="55" t="s">
-        <v>451</v>
+        <v>528</v>
       </c>
       <c r="F56" s="54" t="s">
         <v>77</v>
@@ -7991,7 +8120,7 @@
       <c r="G56" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H56" s="196" t="s">
+      <c r="H56" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I56" s="20" t="s">
@@ -8017,7 +8146,7 @@
       <c r="S56" s="60"/>
       <c r="T56" s="150"/>
       <c r="U56" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V56" s="180"/>
       <c r="W56" s="61"/>
@@ -8034,7 +8163,7 @@
     </row>
     <row r="57" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A57" s="39" t="s">
-        <v>459</v>
+        <v>476</v>
       </c>
       <c r="B57" s="53" t="s">
         <v>37</v>
@@ -8046,7 +8175,7 @@
         <v>285</v>
       </c>
       <c r="E57" s="55" t="s">
-        <v>451</v>
+        <v>529</v>
       </c>
       <c r="F57" s="54" t="s">
         <v>77</v>
@@ -8054,7 +8183,7 @@
       <c r="G57" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H57" s="196" t="s">
+      <c r="H57" s="210" t="s">
         <v>357</v>
       </c>
       <c r="I57" s="20" t="s">
@@ -8080,7 +8209,7 @@
       <c r="S57" s="60"/>
       <c r="T57" s="150"/>
       <c r="U57" s="21" t="s">
-        <v>464</v>
+        <v>481</v>
       </c>
       <c r="V57" s="180"/>
       <c r="W57" s="61"/>
@@ -8099,14 +8228,14 @@
       <c r="A58" s="39"/>
       <c r="B58" s="53"/>
       <c r="C58" s="54"/>
-      <c r="D58" s="29"/>
+      <c r="D58" s="54"/>
       <c r="E58" s="55"/>
       <c r="F58" s="54"/>
       <c r="G58" s="56"/>
-      <c r="H58" s="196"/>
-      <c r="I58" s="20"/>
+      <c r="H58" s="53"/>
+      <c r="I58" s="57"/>
       <c r="J58" s="53"/>
-      <c r="K58" s="28"/>
+      <c r="K58" s="57"/>
       <c r="L58" s="149"/>
       <c r="M58" s="58"/>
       <c r="N58" s="57"/>
@@ -8116,10 +8245,10 @@
       <c r="R58" s="59"/>
       <c r="S58" s="60"/>
       <c r="T58" s="150"/>
-      <c r="U58" s="21"/>
+      <c r="U58" s="164"/>
       <c r="V58" s="180"/>
       <c r="W58" s="61"/>
-      <c r="X58" s="21"/>
+      <c r="X58" s="61"/>
       <c r="Y58" s="151"/>
       <c r="Z58" s="62"/>
       <c r="AA58" s="62"/>
@@ -8132,14 +8261,14 @@
       <c r="A59" s="39"/>
       <c r="B59" s="53"/>
       <c r="C59" s="54"/>
-      <c r="D59" s="29"/>
+      <c r="D59" s="54"/>
       <c r="E59" s="55"/>
       <c r="F59" s="54"/>
       <c r="G59" s="56"/>
-      <c r="H59" s="196"/>
-      <c r="I59" s="20"/>
+      <c r="H59" s="53"/>
+      <c r="I59" s="57"/>
       <c r="J59" s="53"/>
-      <c r="K59" s="28"/>
+      <c r="K59" s="57"/>
       <c r="L59" s="149"/>
       <c r="M59" s="58"/>
       <c r="N59" s="57"/>
@@ -8149,10 +8278,10 @@
       <c r="R59" s="59"/>
       <c r="S59" s="60"/>
       <c r="T59" s="150"/>
-      <c r="U59" s="21"/>
+      <c r="U59" s="164"/>
       <c r="V59" s="180"/>
       <c r="W59" s="61"/>
-      <c r="X59" s="21"/>
+      <c r="X59" s="61"/>
       <c r="Y59" s="151"/>
       <c r="Z59" s="62"/>
       <c r="AA59" s="62"/>
@@ -8165,14 +8294,14 @@
       <c r="A60" s="39"/>
       <c r="B60" s="53"/>
       <c r="C60" s="54"/>
-      <c r="D60" s="29"/>
+      <c r="D60" s="54"/>
       <c r="E60" s="55"/>
       <c r="F60" s="54"/>
       <c r="G60" s="56"/>
-      <c r="H60" s="196"/>
-      <c r="I60" s="20"/>
+      <c r="H60" s="53"/>
+      <c r="I60" s="57"/>
       <c r="J60" s="53"/>
-      <c r="K60" s="28"/>
+      <c r="K60" s="57"/>
       <c r="L60" s="149"/>
       <c r="M60" s="58"/>
       <c r="N60" s="57"/>
@@ -8182,10 +8311,10 @@
       <c r="R60" s="59"/>
       <c r="S60" s="60"/>
       <c r="T60" s="150"/>
-      <c r="U60" s="21"/>
+      <c r="U60" s="164"/>
       <c r="V60" s="180"/>
       <c r="W60" s="61"/>
-      <c r="X60" s="21"/>
+      <c r="X60" s="61"/>
       <c r="Y60" s="151"/>
       <c r="Z60" s="62"/>
       <c r="AA60" s="62"/>
@@ -8198,14 +8327,14 @@
       <c r="A61" s="39"/>
       <c r="B61" s="53"/>
       <c r="C61" s="54"/>
-      <c r="D61" s="29"/>
+      <c r="D61" s="54"/>
       <c r="E61" s="55"/>
       <c r="F61" s="54"/>
       <c r="G61" s="56"/>
-      <c r="H61" s="196"/>
-      <c r="I61" s="20"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="57"/>
       <c r="J61" s="53"/>
-      <c r="K61" s="28"/>
+      <c r="K61" s="57"/>
       <c r="L61" s="149"/>
       <c r="M61" s="58"/>
       <c r="N61" s="57"/>
@@ -8215,10 +8344,10 @@
       <c r="R61" s="59"/>
       <c r="S61" s="60"/>
       <c r="T61" s="150"/>
-      <c r="U61" s="21"/>
+      <c r="U61" s="164"/>
       <c r="V61" s="180"/>
       <c r="W61" s="61"/>
-      <c r="X61" s="21"/>
+      <c r="X61" s="61"/>
       <c r="Y61" s="151"/>
       <c r="Z61" s="62"/>
       <c r="AA61" s="62"/>
@@ -8231,14 +8360,14 @@
       <c r="A62" s="39"/>
       <c r="B62" s="53"/>
       <c r="C62" s="54"/>
-      <c r="D62" s="29"/>
+      <c r="D62" s="54"/>
       <c r="E62" s="55"/>
       <c r="F62" s="54"/>
       <c r="G62" s="56"/>
-      <c r="H62" s="196"/>
-      <c r="I62" s="20"/>
+      <c r="H62" s="53"/>
+      <c r="I62" s="57"/>
       <c r="J62" s="53"/>
-      <c r="K62" s="28"/>
+      <c r="K62" s="57"/>
       <c r="L62" s="149"/>
       <c r="M62" s="58"/>
       <c r="N62" s="57"/>
@@ -8248,10 +8377,10 @@
       <c r="R62" s="59"/>
       <c r="S62" s="60"/>
       <c r="T62" s="150"/>
-      <c r="U62" s="21"/>
+      <c r="U62" s="164"/>
       <c r="V62" s="180"/>
       <c r="W62" s="61"/>
-      <c r="X62" s="21"/>
+      <c r="X62" s="61"/>
       <c r="Y62" s="151"/>
       <c r="Z62" s="62"/>
       <c r="AA62" s="62"/>
@@ -8264,14 +8393,14 @@
       <c r="A63" s="39"/>
       <c r="B63" s="53"/>
       <c r="C63" s="54"/>
-      <c r="D63" s="29"/>
+      <c r="D63" s="54"/>
       <c r="E63" s="55"/>
       <c r="F63" s="54"/>
       <c r="G63" s="56"/>
-      <c r="H63" s="196"/>
-      <c r="I63" s="20"/>
+      <c r="H63" s="53"/>
+      <c r="I63" s="57"/>
       <c r="J63" s="53"/>
-      <c r="K63" s="28"/>
+      <c r="K63" s="57"/>
       <c r="L63" s="149"/>
       <c r="M63" s="58"/>
       <c r="N63" s="57"/>
@@ -8281,10 +8410,10 @@
       <c r="R63" s="59"/>
       <c r="S63" s="60"/>
       <c r="T63" s="150"/>
-      <c r="U63" s="21"/>
+      <c r="U63" s="164"/>
       <c r="V63" s="180"/>
       <c r="W63" s="61"/>
-      <c r="X63" s="21"/>
+      <c r="X63" s="61"/>
       <c r="Y63" s="151"/>
       <c r="Z63" s="62"/>
       <c r="AA63" s="62"/>
@@ -8297,14 +8426,14 @@
       <c r="A64" s="39"/>
       <c r="B64" s="53"/>
       <c r="C64" s="54"/>
-      <c r="D64" s="29"/>
+      <c r="D64" s="54"/>
       <c r="E64" s="55"/>
       <c r="F64" s="54"/>
       <c r="G64" s="56"/>
-      <c r="H64" s="196"/>
-      <c r="I64" s="20"/>
+      <c r="H64" s="53"/>
+      <c r="I64" s="57"/>
       <c r="J64" s="53"/>
-      <c r="K64" s="28"/>
+      <c r="K64" s="57"/>
       <c r="L64" s="149"/>
       <c r="M64" s="58"/>
       <c r="N64" s="57"/>
@@ -8314,10 +8443,10 @@
       <c r="R64" s="59"/>
       <c r="S64" s="60"/>
       <c r="T64" s="150"/>
-      <c r="U64" s="21"/>
+      <c r="U64" s="164"/>
       <c r="V64" s="180"/>
       <c r="W64" s="61"/>
-      <c r="X64" s="21"/>
+      <c r="X64" s="61"/>
       <c r="Y64" s="151"/>
       <c r="Z64" s="62"/>
       <c r="AA64" s="62"/>
@@ -8330,14 +8459,14 @@
       <c r="A65" s="39"/>
       <c r="B65" s="53"/>
       <c r="C65" s="54"/>
-      <c r="D65" s="29"/>
+      <c r="D65" s="54"/>
       <c r="E65" s="55"/>
       <c r="F65" s="54"/>
       <c r="G65" s="56"/>
-      <c r="H65" s="196"/>
-      <c r="I65" s="20"/>
+      <c r="H65" s="53"/>
+      <c r="I65" s="57"/>
       <c r="J65" s="53"/>
-      <c r="K65" s="28"/>
+      <c r="K65" s="57"/>
       <c r="L65" s="149"/>
       <c r="M65" s="58"/>
       <c r="N65" s="57"/>
@@ -8347,10 +8476,10 @@
       <c r="R65" s="59"/>
       <c r="S65" s="60"/>
       <c r="T65" s="150"/>
-      <c r="U65" s="21"/>
+      <c r="U65" s="164"/>
       <c r="V65" s="180"/>
       <c r="W65" s="61"/>
-      <c r="X65" s="21"/>
+      <c r="X65" s="61"/>
       <c r="Y65" s="151"/>
       <c r="Z65" s="62"/>
       <c r="AA65" s="62"/>
@@ -8363,14 +8492,14 @@
       <c r="A66" s="39"/>
       <c r="B66" s="53"/>
       <c r="C66" s="54"/>
-      <c r="D66" s="29"/>
+      <c r="D66" s="54"/>
       <c r="E66" s="55"/>
       <c r="F66" s="54"/>
       <c r="G66" s="56"/>
-      <c r="H66" s="196"/>
-      <c r="I66" s="20"/>
+      <c r="H66" s="53"/>
+      <c r="I66" s="57"/>
       <c r="J66" s="53"/>
-      <c r="K66" s="28"/>
+      <c r="K66" s="57"/>
       <c r="L66" s="149"/>
       <c r="M66" s="58"/>
       <c r="N66" s="57"/>
@@ -8380,10 +8509,10 @@
       <c r="R66" s="59"/>
       <c r="S66" s="60"/>
       <c r="T66" s="150"/>
-      <c r="U66" s="21"/>
+      <c r="U66" s="164"/>
       <c r="V66" s="180"/>
       <c r="W66" s="61"/>
-      <c r="X66" s="21"/>
+      <c r="X66" s="61"/>
       <c r="Y66" s="151"/>
       <c r="Z66" s="62"/>
       <c r="AA66" s="62"/>
@@ -19417,7 +19546,7 @@
       <c r="AB428" s="163"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="l+y1VlLLNhBlFLcXnJJn7P5Sov2yGUvpSG7Mdwgd74Ts5el74bNvdYPmgG2T68BU5+54kQRpZmCsuu/NQKh+xQ==" saltValue="6iq1S6nt8WB98pxcY/Mjmw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="W9:X9"/>
     <mergeCell ref="A9:K9"/>
@@ -19530,15 +19659,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DB8F3B2-ED07-314E-8B12-E986A210F9E2}">
           <x14:formula1>
-            <xm:f>'Drop down lists'!$K$3:$K$5</xm:f>
+            <xm:f>'Drop down lists'!$K$3:$K$6</xm:f>
           </x14:formula1>
           <xm:sqref>W15:W394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Make sure the information matches the valid Application tags in the information tab" xr:uid="{4B818C0C-591E-D74F-998D-F811DA860665}">
           <x14:formula1>
-            <xm:f>'Drop down lists'!$C$3:$C$40</xm:f>
+            <xm:f>'Drop down lists'!$C$3:$C$41</xm:f>
           </x14:formula1>
-          <xm:sqref>D15:D63 D67:D394</xm:sqref>
+          <xm:sqref>D15:D394</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -19553,8 +19682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AL103"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C40" sqref="C4:C40"/>
+    <sheetView topLeftCell="E2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -19621,7 +19750,7 @@
         <v>284</v>
       </c>
       <c r="K2" s="26" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="L2" s="27" t="s">
         <v>80</v>
@@ -19667,7 +19796,7 @@
         <v>355</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>15</v>
@@ -19691,7 +19820,7 @@
         <v>300</v>
       </c>
       <c r="K3" s="173" t="s">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="L3" s="167" t="s">
         <v>27</v>
@@ -19745,7 +19874,7 @@
         <v>301</v>
       </c>
       <c r="K4" s="173" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="L4" s="168" t="s">
         <v>28</v>
@@ -19792,8 +19921,8 @@
       <c r="J5" s="173" t="s">
         <v>77</v>
       </c>
-      <c r="K5" s="173" t="s">
-        <v>423</v>
+      <c r="K5" s="196" t="s">
+        <v>429</v>
       </c>
       <c r="L5" s="168" t="s">
         <v>29</v>
@@ -19832,6 +19961,9 @@
       <c r="I6" s="30" t="s">
         <v>102</v>
       </c>
+      <c r="K6" s="173" t="s">
+        <v>419</v>
+      </c>
       <c r="L6" s="167" t="s">
         <v>30</v>
       </c>
@@ -19996,7 +20128,7 @@
     <row r="11" spans="1:38">
       <c r="A11" s="31"/>
       <c r="C11" s="29" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="20" t="s">
@@ -20209,7 +20341,7 @@
       <c r="A17" s="31"/>
       <c r="B17" s="33"/>
       <c r="C17" s="29" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="20" t="s">
@@ -20243,7 +20375,7 @@
       <c r="A18" s="31"/>
       <c r="B18" s="33"/>
       <c r="C18" s="29" t="s">
-        <v>396</v>
+        <v>431</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="20" t="s">
@@ -20277,7 +20409,7 @@
       <c r="A19" s="31"/>
       <c r="B19" s="33"/>
       <c r="C19" s="29" t="s">
-        <v>397</v>
+        <v>432</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="20" t="s">
@@ -20311,7 +20443,7 @@
       <c r="A20" s="31"/>
       <c r="B20" s="33"/>
       <c r="C20" s="29" t="s">
-        <v>398</v>
+        <v>433</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="20" t="s">
@@ -20345,7 +20477,7 @@
       <c r="A21" s="31"/>
       <c r="B21" s="33"/>
       <c r="C21" s="29" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="20" t="s">
@@ -20379,7 +20511,7 @@
       <c r="A22" s="31"/>
       <c r="B22" s="33"/>
       <c r="C22" s="29" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="20" t="s">
@@ -20413,7 +20545,7 @@
       <c r="A23" s="31"/>
       <c r="B23" s="33"/>
       <c r="C23" s="29" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="20" t="s">
@@ -20444,7 +20576,7 @@
       <c r="A24" s="31"/>
       <c r="B24" s="33"/>
       <c r="C24" s="29" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="20" t="s">
@@ -20475,7 +20607,7 @@
       <c r="A25" s="31"/>
       <c r="B25" s="33"/>
       <c r="C25" s="29" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="20" t="s">
@@ -20506,7 +20638,7 @@
       <c r="A26" s="31"/>
       <c r="B26" s="33"/>
       <c r="C26" s="29" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="20" t="s">
@@ -20537,7 +20669,7 @@
       <c r="A27" s="31"/>
       <c r="B27" s="33"/>
       <c r="C27" s="29" t="s">
-        <v>249</v>
+        <v>404</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="20" t="s">
@@ -20568,7 +20700,7 @@
       <c r="A28" s="31"/>
       <c r="B28" s="33"/>
       <c r="C28" s="29" t="s">
-        <v>408</v>
+        <v>249</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="20" t="s">
@@ -20599,7 +20731,7 @@
       <c r="A29" s="31"/>
       <c r="B29" s="33"/>
       <c r="C29" s="29" t="s">
-        <v>364</v>
+        <v>405</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="20" t="s">
@@ -20630,7 +20762,7 @@
       <c r="A30" s="31"/>
       <c r="B30" s="33"/>
       <c r="C30" s="29" t="s">
-        <v>409</v>
+        <v>364</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="20" t="s">
@@ -20661,7 +20793,7 @@
       <c r="A31" s="21"/>
       <c r="B31" s="33"/>
       <c r="C31" s="29" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="20" t="s">
@@ -20692,7 +20824,7 @@
       <c r="A32" s="21"/>
       <c r="B32" s="33"/>
       <c r="C32" s="29" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="20" t="s">
@@ -20723,7 +20855,7 @@
       <c r="A33" s="21"/>
       <c r="B33" s="33"/>
       <c r="C33" s="29" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="20" t="s">
@@ -20754,7 +20886,7 @@
       <c r="A34" s="21"/>
       <c r="B34" s="33"/>
       <c r="C34" s="29" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="20" t="s">
@@ -20785,7 +20917,7 @@
       <c r="A35" s="21"/>
       <c r="B35" s="33"/>
       <c r="C35" s="29" t="s">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="20" t="s">
@@ -20816,7 +20948,7 @@
       <c r="A36" s="21"/>
       <c r="B36" s="33"/>
       <c r="C36" s="29" t="s">
-        <v>414</v>
+        <v>401</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="20" t="s">
@@ -20847,7 +20979,7 @@
       <c r="A37" s="21"/>
       <c r="B37" s="33"/>
       <c r="C37" s="29" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="20" t="s">
@@ -20878,7 +21010,7 @@
       <c r="A38" s="21"/>
       <c r="B38" s="33"/>
       <c r="C38" s="29" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="20" t="s">
@@ -20909,7 +21041,7 @@
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="29" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="20" t="s">
@@ -20940,7 +21072,7 @@
       <c r="A40" s="21"/>
       <c r="B40" s="21"/>
       <c r="C40" s="29" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="20" t="s">
@@ -20970,7 +21102,9 @@
     <row r="41" spans="1:22">
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
+      <c r="C41" s="29" t="s">
+        <v>415</v>
+      </c>
       <c r="D41" s="21"/>
       <c r="E41" s="20" t="s">
         <v>74</v>
@@ -22155,6 +22289,7 @@
     <row r="86" spans="1:22">
       <c r="A86" s="21"/>
       <c r="B86" s="21"/>
+      <c r="C86" s="21"/>
       <c r="D86" s="21"/>
       <c r="E86" s="20" t="s">
         <v>256</v>
@@ -22589,7 +22724,7 @@
       <c r="V103" s="21"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6q4ec6/bYgp+udUAxk2xZ4MDN+ZK9oNi/aJGljVPVvwjuH/ESpK/mB6mudDLq0yMJfoPEVCglmSNkUoP5kFA0A==" saltValue="H9J7NbCgUIEEH+c/MMMNxg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="OJFtPcw1Smz57zpSg0eibTEQTykzI9svcg7GftP2lBA7QFS7NCmOzJsoXM5Eo+ed1/q0N92EfhKxmpnlEtGw+Q==" saltValue="k9ec4vayQ7/FAqum2SCTzA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
remove unused panels from test fixture
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.17.mip_balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.17.mip_balsamic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1FBD62-4DB2-4045-BC4E-C9EC825F924D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1701047-6DB5-5143-A4C8-ECB0D81DE65D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="1180" windowWidth="33060" windowHeight="25340" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1600" yWindow="460" windowWidth="47900" windowHeight="27380" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="5" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="482">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -1066,27 +1066,12 @@
     <t>Gene List</t>
   </si>
   <si>
-    <t>16PDEL</t>
-  </si>
-  <si>
-    <t>AD</t>
-  </si>
-  <si>
-    <t>AD-1.0-141202</t>
-  </si>
-  <si>
     <t>ATX</t>
   </si>
   <si>
     <t>CILM</t>
   </si>
   <si>
-    <t>CM</t>
-  </si>
-  <si>
-    <t>CNM</t>
-  </si>
-  <si>
     <t>CTD</t>
   </si>
   <si>
@@ -1157,9 +1142,6 @@
   </si>
   <si>
     <t>PEDHEP</t>
-  </si>
-  <si>
-    <t>bindvev</t>
   </si>
   <si>
     <t>panel1</t>
@@ -1698,9 +1680,6 @@
     <t>Added skin as a sample source</t>
   </si>
   <si>
-    <t>Removed panels: SHANK1, MTM1, MLD, horsel, SCN, MOYA, SHP, ORO, PAF1</t>
-  </si>
-  <si>
     <t>Updated Application tags</t>
   </si>
   <si>
@@ -1791,6 +1770,12 @@
     <t>EXTTTTR040</t>
   </si>
   <si>
+    <t>bindevev</t>
+  </si>
+  <si>
+    <t>Removed panels: SHANK1, MTM1, MLD, horsel, SCN, MOYA, SHP, ORO, PAF1, 16PDEL, AD, AD-1.0141202, CM, CNM</t>
+  </si>
+  <si>
     <t>whole-genome-1</t>
   </si>
   <si>
@@ -1920,21 +1905,6 @@
     <t>gene-list-test-4</t>
   </si>
   <si>
-    <t>gene-list-test-5</t>
-  </si>
-  <si>
-    <t>gene-list-test-6</t>
-  </si>
-  <si>
-    <t>gene-list-test-7</t>
-  </si>
-  <si>
-    <t>gene-list-test-8</t>
-  </si>
-  <si>
-    <t>gene-list-test-9</t>
-  </si>
-  <si>
     <t>plate</t>
   </si>
   <si>
@@ -1953,16 +1923,16 @@
     <t>other (specify in comment field)</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
     <t>Nuclease free water</t>
   </si>
   <si>
     <t>Tris-HCl (pH 8-8.5)</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>comment</t>
   </si>
 </sst>
 </file>
@@ -4330,7 +4300,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4374,7 +4344,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4398,8 +4368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD6"/>
+    <sheetView topLeftCell="A6" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4416,7 +4386,7 @@
         <v>22</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="2"/>
@@ -4428,28 +4398,28 @@
       <c r="D2" s="9"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="13" hidden="1" customHeight="1">
+    <row r="3" spans="1:5" ht="14" hidden="1" customHeight="1">
       <c r="A3" s="12"/>
       <c r="B3" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="170">
-        <v>43605</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" hidden="1">
+        <v>43612</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="12" hidden="1" customHeight="1">
       <c r="A4" s="12"/>
       <c r="B4" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>26</v>
@@ -4458,8 +4428,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14" hidden="1" customHeight="1"/>
-    <row r="6" spans="1:5" ht="14" hidden="1" customHeight="1"/>
+    <row r="5" spans="1:5" ht="12" hidden="1" customHeight="1"/>
     <row r="8" spans="1:5" ht="12" customHeight="1"/>
     <row r="9" spans="1:5" ht="14" customHeight="1"/>
     <row r="14" spans="1:5" ht="19">
@@ -4474,27 +4443,27 @@
     </row>
     <row r="16" spans="1:5" ht="14">
       <c r="A16" s="15" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="14">
       <c r="A17" s="15" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="14">
       <c r="A18" s="15" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="14">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="28">
       <c r="A19" s="15" t="s">
-        <v>417</v>
+        <v>428</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="14">
       <c r="A20" s="15" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="16">
@@ -4514,12 +4483,12 @@
     </row>
     <row r="26" spans="1:1" ht="28">
       <c r="A26" s="35" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="98">
       <c r="A27" s="35" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="36" customHeight="1">
@@ -4529,12 +4498,12 @@
     </row>
     <row r="29" spans="1:1" ht="56">
       <c r="A29" s="35" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="27" customHeight="1">
       <c r="A30" s="35" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="28">
@@ -4549,7 +4518,7 @@
     </row>
     <row r="33" spans="1:5" ht="52" customHeight="1">
       <c r="A33" s="34" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C33" s="15"/>
       <c r="E33" s="15"/>
@@ -4580,7 +4549,7 @@
     </row>
     <row r="39" spans="1:5" ht="28">
       <c r="A39" s="34" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="C39" s="15"/>
       <c r="E39" s="15"/>
@@ -4598,42 +4567,42 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="19" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="37" customHeight="1">
       <c r="A44" s="34" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="28" customHeight="1">
       <c r="A45" s="34" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="26" customHeight="1">
       <c r="A46" s="34" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="29" customHeight="1">
       <c r="A47" s="34" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="19" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="28">
       <c r="A50" s="34" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="19" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="52" spans="1:1">
@@ -4641,7 +4610,7 @@
     </row>
     <row r="53" spans="1:1" ht="42">
       <c r="A53" s="176" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="54" spans="1:1">
@@ -4649,7 +4618,7 @@
     </row>
     <row r="55" spans="1:1" ht="28">
       <c r="A55" s="34" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="56" spans="1:1">
@@ -4657,22 +4626,22 @@
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="19" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="14">
       <c r="A59" s="34" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="28" customHeight="1">
       <c r="A60" s="36" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="28" customHeight="1">
       <c r="A61" s="36" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="62" spans="1:1">
@@ -4733,7 +4702,7 @@
       <c r="A83" s="15"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="4hxgLibnT+qvSFmfmjUMHWExefFntKM8u3f5i5xQxyRSRuhWb0bB907+FMarbA98InnIUuJdSJ1l39nY4mbIbg==" saltValue="MY1gDBRgAtdf2sAb/ggfWQ==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
     <hyperlink ref="A14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
@@ -4756,7 +4725,7 @@
   <dimension ref="A1:AE428"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -5070,23 +5039,23 @@
       <c r="N9" s="202"/>
       <c r="O9" s="99"/>
       <c r="P9" s="204" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="Q9" s="205"/>
       <c r="R9" s="205"/>
       <c r="S9" s="206"/>
       <c r="T9" s="100"/>
       <c r="U9" s="183" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="V9" s="101"/>
       <c r="W9" s="197" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="X9" s="197"/>
       <c r="Y9" s="101"/>
       <c r="Z9" s="207" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="AA9" s="208"/>
       <c r="AB9" s="209"/>
@@ -5174,7 +5143,7 @@
       </c>
       <c r="O11" s="112"/>
       <c r="P11" s="109" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="Q11" s="191" t="s">
         <v>291</v>
@@ -5187,24 +5156,24 @@
       </c>
       <c r="T11" s="114"/>
       <c r="U11" s="194" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="V11" s="179"/>
       <c r="W11" s="195" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="X11" s="115" t="s">
         <v>278</v>
       </c>
       <c r="Y11" s="116"/>
       <c r="Z11" s="115" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="AA11" s="115" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="AB11" s="115" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="AC11" s="117"/>
       <c r="AD11" s="106" t="s">
@@ -5305,24 +5274,24 @@
       </c>
       <c r="T13" s="138"/>
       <c r="U13" s="140" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="V13" s="181"/>
       <c r="W13" s="140" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="X13" s="140" t="s">
         <v>296</v>
       </c>
       <c r="Y13" s="141"/>
       <c r="Z13" s="139" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="AA13" s="142" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="AB13" s="142" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="AC13" s="143"/>
       <c r="AD13" s="113" t="s">
@@ -5369,19 +5338,19 @@
     </row>
     <row r="15" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A15" s="55" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B15" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>285</v>
       </c>
       <c r="E15" s="55" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F15" s="54" t="s">
         <v>15</v>
@@ -5403,31 +5372,31 @@
       </c>
       <c r="L15" s="149"/>
       <c r="M15" s="58" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="N15" s="57" t="s">
         <v>27</v>
       </c>
       <c r="O15" s="149"/>
       <c r="P15" s="30" t="s">
-        <v>303</v>
+        <v>326</v>
       </c>
       <c r="Q15" s="56" t="s">
         <v>300</v>
       </c>
       <c r="R15" s="55" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="S15" s="211" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="T15" s="150"/>
       <c r="U15" s="21" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="V15" s="180"/>
       <c r="W15" s="61" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="X15" s="21">
         <v>5</v>
@@ -5440,31 +5409,31 @@
         <v>2</v>
       </c>
       <c r="AB15" s="63" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="AC15" s="152"/>
       <c r="AD15" s="58" t="s">
-        <v>490</v>
+        <v>478</v>
       </c>
       <c r="AE15" s="58" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
     </row>
     <row r="16" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A16" s="55" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="B16" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>290</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F16" s="54" t="s">
         <v>16</v>
@@ -5489,7 +5458,7 @@
       <c r="N16" s="57"/>
       <c r="O16" s="149"/>
       <c r="P16" s="30" t="s">
-        <v>304</v>
+        <v>325</v>
       </c>
       <c r="Q16" s="56" t="s">
         <v>301</v>
@@ -5498,7 +5467,7 @@
       <c r="S16" s="60"/>
       <c r="T16" s="150"/>
       <c r="U16" s="33" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="V16" s="180"/>
       <c r="W16" s="61"/>
@@ -5509,7 +5478,7 @@
       <c r="Z16" s="62"/>
       <c r="AA16" s="62"/>
       <c r="AB16" s="63" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="AC16" s="152"/>
       <c r="AD16" s="58"/>
@@ -5517,19 +5486,19 @@
     </row>
     <row r="17" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A17" s="55" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B17" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>286</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F17" s="54" t="s">
         <v>15</v>
@@ -5554,7 +5523,7 @@
       <c r="N17" s="57"/>
       <c r="O17" s="149"/>
       <c r="P17" s="30" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="Q17" s="56" t="s">
         <v>77</v>
@@ -5563,7 +5532,7 @@
       <c r="S17" s="60"/>
       <c r="T17" s="150"/>
       <c r="U17" s="21" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="V17" s="180"/>
       <c r="W17" s="61"/>
@@ -5580,19 +5549,19 @@
     </row>
     <row r="18" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A18" s="55" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="B18" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>287</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F18" s="54" t="s">
         <v>77</v>
@@ -5617,7 +5586,7 @@
       <c r="N18" s="57"/>
       <c r="O18" s="149"/>
       <c r="P18" s="30" t="s">
-        <v>331</v>
+        <v>427</v>
       </c>
       <c r="Q18" s="56" t="s">
         <v>77</v>
@@ -5626,7 +5595,7 @@
       <c r="S18" s="60"/>
       <c r="T18" s="150"/>
       <c r="U18" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V18" s="180"/>
       <c r="W18" s="61"/>
@@ -5643,19 +5612,19 @@
     </row>
     <row r="19" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A19" s="55" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B19" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D19" s="29" t="s">
         <v>288</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F19" s="54" t="s">
         <v>77</v>
@@ -5664,7 +5633,7 @@
         <v>93</v>
       </c>
       <c r="H19" s="41" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>102</v>
@@ -5680,7 +5649,7 @@
       <c r="N19" s="57"/>
       <c r="O19" s="149"/>
       <c r="P19" s="30" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
       <c r="Q19" s="56" t="s">
         <v>77</v>
@@ -5689,7 +5658,7 @@
       <c r="S19" s="60"/>
       <c r="T19" s="150"/>
       <c r="U19" s="21" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
       <c r="V19" s="180"/>
       <c r="W19" s="61"/>
@@ -5706,19 +5675,19 @@
     </row>
     <row r="20" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A20" s="55" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="B20" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D20" s="29" t="s">
         <v>289</v>
       </c>
       <c r="E20" s="55" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F20" s="54" t="s">
         <v>77</v>
@@ -5743,7 +5712,7 @@
       <c r="N20" s="57"/>
       <c r="O20" s="149"/>
       <c r="P20" s="30" t="s">
-        <v>306</v>
+        <v>333</v>
       </c>
       <c r="Q20" s="56" t="s">
         <v>77</v>
@@ -5752,7 +5721,7 @@
       <c r="S20" s="60"/>
       <c r="T20" s="150"/>
       <c r="U20" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V20" s="180"/>
       <c r="W20" s="61"/>
@@ -5769,19 +5738,19 @@
     </row>
     <row r="21" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A21" s="55" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B21" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="E21" s="55" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F21" s="54" t="s">
         <v>77</v>
@@ -5806,7 +5775,7 @@
       <c r="N21" s="57"/>
       <c r="O21" s="149"/>
       <c r="P21" s="30" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="Q21" s="56" t="s">
         <v>77</v>
@@ -5815,7 +5784,7 @@
       <c r="S21" s="60"/>
       <c r="T21" s="150"/>
       <c r="U21" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V21" s="180"/>
       <c r="W21" s="61"/>
@@ -5832,19 +5801,19 @@
     </row>
     <row r="22" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A22" s="55" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="B22" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F22" s="54" t="s">
         <v>77</v>
@@ -5868,8 +5837,8 @@
       <c r="M22" s="58"/>
       <c r="N22" s="57"/>
       <c r="O22" s="149"/>
-      <c r="P22" s="30" t="s">
-        <v>307</v>
+      <c r="P22" s="165" t="s">
+        <v>369</v>
       </c>
       <c r="Q22" s="56" t="s">
         <v>77</v>
@@ -5878,7 +5847,7 @@
       <c r="S22" s="60"/>
       <c r="T22" s="150"/>
       <c r="U22" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V22" s="180"/>
       <c r="W22" s="61"/>
@@ -5895,19 +5864,19 @@
     </row>
     <row r="23" spans="1:31" ht="25" customHeight="1">
       <c r="A23" s="55" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="B23" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="E23" s="55" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F23" s="54" t="s">
         <v>77</v>
@@ -5932,7 +5901,7 @@
       <c r="N23" s="57"/>
       <c r="O23" s="149"/>
       <c r="P23" s="30" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="Q23" s="56" t="s">
         <v>77</v>
@@ -5941,7 +5910,7 @@
       <c r="S23" s="60"/>
       <c r="T23" s="150"/>
       <c r="U23" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V23" s="180"/>
       <c r="W23" s="61"/>
@@ -5958,19 +5927,19 @@
     </row>
     <row r="24" spans="1:31" ht="25" customHeight="1">
       <c r="A24" s="55" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="B24" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C24" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F24" s="54" t="s">
         <v>77</v>
@@ -5979,7 +5948,7 @@
         <v>93</v>
       </c>
       <c r="H24" s="210" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>102</v>
@@ -5995,7 +5964,7 @@
       <c r="N24" s="57"/>
       <c r="O24" s="149"/>
       <c r="P24" s="30" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="Q24" s="56" t="s">
         <v>77</v>
@@ -6004,7 +5973,7 @@
       <c r="S24" s="60"/>
       <c r="T24" s="150"/>
       <c r="U24" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V24" s="180"/>
       <c r="W24" s="61"/>
@@ -6021,19 +5990,19 @@
     </row>
     <row r="25" spans="1:31" ht="25" customHeight="1">
       <c r="A25" s="55" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B25" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="E25" s="55" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F25" s="54" t="s">
         <v>77</v>
@@ -6042,7 +6011,7 @@
         <v>93</v>
       </c>
       <c r="H25" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I25" s="20" t="s">
         <v>102</v>
@@ -6058,7 +6027,7 @@
       <c r="N25" s="57"/>
       <c r="O25" s="149"/>
       <c r="P25" s="30" t="s">
-        <v>339</v>
+        <v>318</v>
       </c>
       <c r="Q25" s="56" t="s">
         <v>77</v>
@@ -6067,11 +6036,11 @@
       <c r="S25" s="60"/>
       <c r="T25" s="150"/>
       <c r="U25" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V25" s="180"/>
       <c r="W25" s="61" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="X25" s="21">
         <v>55</v>
@@ -6086,19 +6055,19 @@
     </row>
     <row r="26" spans="1:31" ht="25" customHeight="1">
       <c r="A26" s="55" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="B26" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="E26" s="55" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F26" s="54" t="s">
         <v>77</v>
@@ -6123,7 +6092,7 @@
       <c r="N26" s="57"/>
       <c r="O26" s="149"/>
       <c r="P26" s="30" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="Q26" s="56" t="s">
         <v>77</v>
@@ -6132,11 +6101,11 @@
       <c r="S26" s="60"/>
       <c r="T26" s="150"/>
       <c r="U26" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V26" s="180"/>
       <c r="W26" s="61" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="X26" s="21">
         <v>60</v>
@@ -6151,19 +6120,19 @@
     </row>
     <row r="27" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A27" s="55" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B27" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="E27" s="55" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F27" s="54" t="s">
         <v>77</v>
@@ -6172,7 +6141,7 @@
         <v>93</v>
       </c>
       <c r="H27" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I27" s="20" t="s">
         <v>102</v>
@@ -6187,8 +6156,8 @@
       <c r="M27" s="58"/>
       <c r="N27" s="57"/>
       <c r="O27" s="149"/>
-      <c r="P27" s="165" t="s">
-        <v>375</v>
+      <c r="P27" s="30" t="s">
+        <v>307</v>
       </c>
       <c r="Q27" s="56" t="s">
         <v>77</v>
@@ -6197,11 +6166,11 @@
       <c r="S27" s="60"/>
       <c r="T27" s="150"/>
       <c r="U27" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V27" s="180"/>
       <c r="W27" s="61" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="X27" s="21">
         <v>65</v>
@@ -6216,19 +6185,19 @@
     </row>
     <row r="28" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A28" s="55" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B28" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C28" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="E28" s="55" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F28" s="54" t="s">
         <v>77</v>
@@ -6237,7 +6206,7 @@
         <v>93</v>
       </c>
       <c r="H28" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I28" s="20" t="s">
         <v>102</v>
@@ -6252,8 +6221,8 @@
       <c r="M28" s="58"/>
       <c r="N28" s="57"/>
       <c r="O28" s="149"/>
-      <c r="P28" s="30" t="s">
-        <v>310</v>
+      <c r="P28" s="165" t="s">
+        <v>367</v>
       </c>
       <c r="Q28" s="56" t="s">
         <v>77</v>
@@ -6262,11 +6231,11 @@
       <c r="S28" s="60"/>
       <c r="T28" s="150"/>
       <c r="U28" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V28" s="180"/>
       <c r="W28" s="61" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="X28" s="21">
         <v>70</v>
@@ -6281,19 +6250,19 @@
     </row>
     <row r="29" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A29" s="55" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B29" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="E29" s="55" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F29" s="54" t="s">
         <v>77</v>
@@ -6302,7 +6271,7 @@
         <v>93</v>
       </c>
       <c r="H29" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I29" s="20" t="s">
         <v>102</v>
@@ -6318,7 +6287,7 @@
       <c r="N29" s="57"/>
       <c r="O29" s="149"/>
       <c r="P29" s="30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Q29" s="56" t="s">
         <v>77</v>
@@ -6327,11 +6296,11 @@
       <c r="S29" s="60"/>
       <c r="T29" s="150"/>
       <c r="U29" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V29" s="180"/>
       <c r="W29" s="61" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="X29" s="21">
         <v>75</v>
@@ -6346,19 +6315,19 @@
     </row>
     <row r="30" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A30" s="55" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B30" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C30" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="E30" s="55" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F30" s="54" t="s">
         <v>77</v>
@@ -6367,7 +6336,7 @@
         <v>93</v>
       </c>
       <c r="H30" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I30" s="20" t="s">
         <v>102</v>
@@ -6383,7 +6352,7 @@
       <c r="N30" s="57"/>
       <c r="O30" s="149"/>
       <c r="P30" s="30" t="s">
-        <v>323</v>
+        <v>365</v>
       </c>
       <c r="Q30" s="56" t="s">
         <v>77</v>
@@ -6392,11 +6361,11 @@
       <c r="S30" s="60"/>
       <c r="T30" s="150"/>
       <c r="U30" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V30" s="180"/>
       <c r="W30" s="61" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="X30" s="21">
         <v>80</v>
@@ -6411,19 +6380,19 @@
     </row>
     <row r="31" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A31" s="55" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="B31" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="E31" s="55" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F31" s="54" t="s">
         <v>77</v>
@@ -6432,7 +6401,7 @@
         <v>93</v>
       </c>
       <c r="H31" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I31" s="20" t="s">
         <v>102</v>
@@ -6448,7 +6417,7 @@
       <c r="N31" s="57"/>
       <c r="O31" s="149"/>
       <c r="P31" s="30" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="Q31" s="56" t="s">
         <v>77</v>
@@ -6457,7 +6426,7 @@
       <c r="S31" s="60"/>
       <c r="T31" s="150"/>
       <c r="U31" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V31" s="180"/>
       <c r="W31" s="61"/>
@@ -6474,19 +6443,19 @@
     </row>
     <row r="32" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A32" s="55" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="B32" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C32" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="E32" s="55" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F32" s="54" t="s">
         <v>77</v>
@@ -6495,7 +6464,7 @@
         <v>93</v>
       </c>
       <c r="H32" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I32" s="20" t="s">
         <v>102</v>
@@ -6511,7 +6480,7 @@
       <c r="N32" s="57"/>
       <c r="O32" s="149"/>
       <c r="P32" s="30" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="Q32" s="56" t="s">
         <v>77</v>
@@ -6520,7 +6489,7 @@
       <c r="S32" s="60"/>
       <c r="T32" s="150"/>
       <c r="U32" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V32" s="180"/>
       <c r="W32" s="61"/>
@@ -6537,19 +6506,19 @@
     </row>
     <row r="33" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A33" s="55" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="B33" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="E33" s="55" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="F33" s="54" t="s">
         <v>77</v>
@@ -6558,7 +6527,7 @@
         <v>93</v>
       </c>
       <c r="H33" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>102</v>
@@ -6573,8 +6542,8 @@
       <c r="M33" s="58"/>
       <c r="N33" s="57"/>
       <c r="O33" s="149"/>
-      <c r="P33" s="165" t="s">
-        <v>373</v>
+      <c r="P33" s="30" t="s">
+        <v>315</v>
       </c>
       <c r="Q33" s="56" t="s">
         <v>77</v>
@@ -6583,7 +6552,7 @@
       <c r="S33" s="60"/>
       <c r="T33" s="150"/>
       <c r="U33" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V33" s="180"/>
       <c r="W33" s="61"/>
@@ -6600,19 +6569,19 @@
     </row>
     <row r="34" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A34" s="55" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="B34" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C34" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="E34" s="55" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F34" s="54" t="s">
         <v>77</v>
@@ -6621,7 +6590,7 @@
         <v>93</v>
       </c>
       <c r="H34" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I34" s="20" t="s">
         <v>102</v>
@@ -6636,8 +6605,8 @@
       <c r="M34" s="58"/>
       <c r="N34" s="57"/>
       <c r="O34" s="149"/>
-      <c r="P34" s="30" t="s">
-        <v>315</v>
+      <c r="P34" s="165" t="s">
+        <v>368</v>
       </c>
       <c r="Q34" s="56" t="s">
         <v>77</v>
@@ -6646,7 +6615,7 @@
       <c r="S34" s="60"/>
       <c r="T34" s="150"/>
       <c r="U34" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V34" s="180"/>
       <c r="W34" s="61"/>
@@ -6663,19 +6632,19 @@
     </row>
     <row r="35" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A35" s="55" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="B35" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C35" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="E35" s="55" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F35" s="54" t="s">
         <v>77</v>
@@ -6684,7 +6653,7 @@
         <v>93</v>
       </c>
       <c r="H35" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I35" s="20" t="s">
         <v>102</v>
@@ -6700,7 +6669,7 @@
       <c r="N35" s="57"/>
       <c r="O35" s="149"/>
       <c r="P35" s="30" t="s">
-        <v>371</v>
+        <v>330</v>
       </c>
       <c r="Q35" s="56" t="s">
         <v>77</v>
@@ -6709,7 +6678,7 @@
       <c r="S35" s="60"/>
       <c r="T35" s="150"/>
       <c r="U35" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V35" s="180"/>
       <c r="W35" s="61"/>
@@ -6726,19 +6695,19 @@
     </row>
     <row r="36" spans="1:31" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A36" s="55" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="B36" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="E36" s="55" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F36" s="54" t="s">
         <v>77</v>
@@ -6747,7 +6716,7 @@
         <v>93</v>
       </c>
       <c r="H36" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I36" s="20" t="s">
         <v>102</v>
@@ -6763,7 +6732,7 @@
       <c r="N36" s="57"/>
       <c r="O36" s="149"/>
       <c r="P36" s="30" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="Q36" s="56" t="s">
         <v>77</v>
@@ -6772,7 +6741,7 @@
       <c r="S36" s="60"/>
       <c r="T36" s="150"/>
       <c r="U36" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V36" s="180"/>
       <c r="W36" s="61"/>
@@ -6789,19 +6758,19 @@
     </row>
     <row r="37" spans="1:31" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A37" s="55" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="B37" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C37" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D37" s="29" t="s">
         <v>249</v>
       </c>
       <c r="E37" s="55" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F37" s="54" t="s">
         <v>77</v>
@@ -6810,7 +6779,7 @@
         <v>93</v>
       </c>
       <c r="H37" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I37" s="20" t="s">
         <v>102</v>
@@ -6826,7 +6795,7 @@
       <c r="N37" s="57"/>
       <c r="O37" s="149"/>
       <c r="P37" s="30" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="Q37" s="56" t="s">
         <v>77</v>
@@ -6835,7 +6804,7 @@
       <c r="S37" s="60"/>
       <c r="T37" s="150"/>
       <c r="U37" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V37" s="180"/>
       <c r="W37" s="61"/>
@@ -6852,19 +6821,19 @@
     </row>
     <row r="38" spans="1:31" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A38" s="55" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B38" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="E38" s="55" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F38" s="54" t="s">
         <v>77</v>
@@ -6873,7 +6842,7 @@
         <v>93</v>
       </c>
       <c r="H38" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I38" s="20" t="s">
         <v>102</v>
@@ -6888,8 +6857,8 @@
       <c r="M38" s="58"/>
       <c r="N38" s="57"/>
       <c r="O38" s="149"/>
-      <c r="P38" s="30" t="s">
-        <v>320</v>
+      <c r="P38" s="165" t="s">
+        <v>366</v>
       </c>
       <c r="Q38" s="56" t="s">
         <v>77</v>
@@ -6898,7 +6867,7 @@
       <c r="S38" s="60"/>
       <c r="T38" s="150"/>
       <c r="U38" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V38" s="180"/>
       <c r="W38" s="61"/>
@@ -6915,19 +6884,19 @@
     </row>
     <row r="39" spans="1:31" ht="25" customHeight="1">
       <c r="A39" s="55" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="B39" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C39" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="E39" s="55" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F39" s="54" t="s">
         <v>77</v>
@@ -6936,7 +6905,7 @@
         <v>93</v>
       </c>
       <c r="H39" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I39" s="20" t="s">
         <v>102</v>
@@ -6951,8 +6920,8 @@
       <c r="M39" s="58"/>
       <c r="N39" s="57"/>
       <c r="O39" s="149"/>
-      <c r="P39" s="165" t="s">
-        <v>374</v>
+      <c r="P39" s="30" t="s">
+        <v>319</v>
       </c>
       <c r="Q39" s="56" t="s">
         <v>77</v>
@@ -6961,7 +6930,7 @@
       <c r="S39" s="60"/>
       <c r="T39" s="150"/>
       <c r="U39" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V39" s="180"/>
       <c r="W39" s="61"/>
@@ -6978,19 +6947,19 @@
     </row>
     <row r="40" spans="1:31" ht="25" customHeight="1">
       <c r="A40" s="55" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="B40" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C40" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="E40" s="55" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F40" s="54" t="s">
         <v>77</v>
@@ -6999,7 +6968,7 @@
         <v>93</v>
       </c>
       <c r="H40" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>102</v>
@@ -7015,7 +6984,7 @@
       <c r="N40" s="57"/>
       <c r="O40" s="149"/>
       <c r="P40" s="30" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="Q40" s="56" t="s">
         <v>77</v>
@@ -7024,7 +6993,7 @@
       <c r="S40" s="60"/>
       <c r="T40" s="150"/>
       <c r="U40" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V40" s="180"/>
       <c r="W40" s="61"/>
@@ -7041,19 +7010,19 @@
     </row>
     <row r="41" spans="1:31" ht="25" customHeight="1">
       <c r="A41" s="55" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="B41" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C41" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="E41" s="55" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F41" s="54" t="s">
         <v>77</v>
@@ -7062,7 +7031,7 @@
         <v>93</v>
       </c>
       <c r="H41" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I41" s="20" t="s">
         <v>102</v>
@@ -7078,7 +7047,7 @@
       <c r="N41" s="57"/>
       <c r="O41" s="149"/>
       <c r="P41" s="30" t="s">
-        <v>340</v>
+        <v>311</v>
       </c>
       <c r="Q41" s="56" t="s">
         <v>77</v>
@@ -7087,7 +7056,7 @@
       <c r="S41" s="60"/>
       <c r="T41" s="150"/>
       <c r="U41" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V41" s="180"/>
       <c r="W41" s="61"/>
@@ -7104,19 +7073,19 @@
     </row>
     <row r="42" spans="1:31" ht="25" customHeight="1">
       <c r="A42" s="55" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B42" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C42" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="E42" s="55" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F42" s="54" t="s">
         <v>77</v>
@@ -7125,7 +7094,7 @@
         <v>93</v>
       </c>
       <c r="H42" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I42" s="20" t="s">
         <v>102</v>
@@ -7141,7 +7110,7 @@
       <c r="N42" s="57"/>
       <c r="O42" s="149"/>
       <c r="P42" s="30" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="Q42" s="56" t="s">
         <v>77</v>
@@ -7150,7 +7119,7 @@
       <c r="S42" s="60"/>
       <c r="T42" s="150"/>
       <c r="U42" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V42" s="180"/>
       <c r="W42" s="61"/>
@@ -7167,19 +7136,19 @@
     </row>
     <row r="43" spans="1:31" ht="25" customHeight="1">
       <c r="A43" s="55" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="B43" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C43" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="E43" s="55" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F43" s="54" t="s">
         <v>77</v>
@@ -7188,7 +7157,7 @@
         <v>93</v>
       </c>
       <c r="H43" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I43" s="20" t="s">
         <v>102</v>
@@ -7203,8 +7172,8 @@
       <c r="M43" s="58"/>
       <c r="N43" s="57"/>
       <c r="O43" s="149"/>
-      <c r="P43" s="165" t="s">
-        <v>372</v>
+      <c r="P43" s="30" t="s">
+        <v>313</v>
       </c>
       <c r="Q43" s="56" t="s">
         <v>77</v>
@@ -7213,7 +7182,7 @@
       <c r="S43" s="60"/>
       <c r="T43" s="150"/>
       <c r="U43" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V43" s="180"/>
       <c r="W43" s="61"/>
@@ -7230,19 +7199,19 @@
     </row>
     <row r="44" spans="1:31" ht="25" customHeight="1">
       <c r="A44" s="55" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="B44" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C44" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="E44" s="55" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="F44" s="54" t="s">
         <v>77</v>
@@ -7251,7 +7220,7 @@
         <v>93</v>
       </c>
       <c r="H44" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I44" s="20" t="s">
         <v>102</v>
@@ -7267,7 +7236,7 @@
       <c r="N44" s="57"/>
       <c r="O44" s="149"/>
       <c r="P44" s="30" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="Q44" s="56" t="s">
         <v>77</v>
@@ -7276,7 +7245,7 @@
       <c r="S44" s="60"/>
       <c r="T44" s="150"/>
       <c r="U44" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V44" s="180"/>
       <c r="W44" s="61"/>
@@ -7293,19 +7262,19 @@
     </row>
     <row r="45" spans="1:31" ht="25" customHeight="1">
       <c r="A45" s="55" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="B45" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C45" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="E45" s="55" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="F45" s="54" t="s">
         <v>77</v>
@@ -7314,7 +7283,7 @@
         <v>93</v>
       </c>
       <c r="H45" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I45" s="20" t="s">
         <v>102</v>
@@ -7330,7 +7299,7 @@
       <c r="N45" s="57"/>
       <c r="O45" s="149"/>
       <c r="P45" s="30" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="Q45" s="56" t="s">
         <v>77</v>
@@ -7339,7 +7308,7 @@
       <c r="S45" s="60"/>
       <c r="T45" s="150"/>
       <c r="U45" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V45" s="180"/>
       <c r="W45" s="61"/>
@@ -7356,19 +7325,19 @@
     </row>
     <row r="46" spans="1:31" ht="25" customHeight="1">
       <c r="A46" s="55" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="B46" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C46" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="E46" s="55" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="F46" s="54" t="s">
         <v>77</v>
@@ -7377,7 +7346,7 @@
         <v>93</v>
       </c>
       <c r="H46" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I46" s="20" t="s">
         <v>102</v>
@@ -7393,7 +7362,7 @@
       <c r="N46" s="57"/>
       <c r="O46" s="149"/>
       <c r="P46" s="30" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="Q46" s="56" t="s">
         <v>77</v>
@@ -7402,7 +7371,7 @@
       <c r="S46" s="60"/>
       <c r="T46" s="150"/>
       <c r="U46" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V46" s="180"/>
       <c r="W46" s="61"/>
@@ -7419,19 +7388,19 @@
     </row>
     <row r="47" spans="1:31" ht="25" customHeight="1">
       <c r="A47" s="55" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="B47" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C47" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="E47" s="55" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="F47" s="54" t="s">
         <v>77</v>
@@ -7440,7 +7409,7 @@
         <v>93</v>
       </c>
       <c r="H47" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I47" s="20" t="s">
         <v>102</v>
@@ -7456,7 +7425,7 @@
       <c r="N47" s="57"/>
       <c r="O47" s="149"/>
       <c r="P47" s="30" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="Q47" s="56" t="s">
         <v>77</v>
@@ -7465,7 +7434,7 @@
       <c r="S47" s="60"/>
       <c r="T47" s="150"/>
       <c r="U47" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V47" s="180"/>
       <c r="W47" s="61"/>
@@ -7482,19 +7451,19 @@
     </row>
     <row r="48" spans="1:31" ht="25" customHeight="1">
       <c r="A48" s="55" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="B48" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C48" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="E48" s="55" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="F48" s="54" t="s">
         <v>77</v>
@@ -7503,7 +7472,7 @@
         <v>93</v>
       </c>
       <c r="H48" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I48" s="20" t="s">
         <v>102</v>
@@ -7519,7 +7488,7 @@
       <c r="N48" s="57"/>
       <c r="O48" s="149"/>
       <c r="P48" s="30" t="s">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="Q48" s="56" t="s">
         <v>77</v>
@@ -7528,7 +7497,7 @@
       <c r="S48" s="60"/>
       <c r="T48" s="150"/>
       <c r="U48" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V48" s="180"/>
       <c r="W48" s="61"/>
@@ -7545,19 +7514,19 @@
     </row>
     <row r="49" spans="1:31" ht="25" customHeight="1">
       <c r="A49" s="39" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="B49" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C49" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="E49" s="55" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="F49" s="54" t="s">
         <v>77</v>
@@ -7566,7 +7535,7 @@
         <v>93</v>
       </c>
       <c r="H49" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I49" s="20" t="s">
         <v>102</v>
@@ -7582,7 +7551,7 @@
       <c r="N49" s="57"/>
       <c r="O49" s="149"/>
       <c r="P49" s="30" t="s">
-        <v>335</v>
+        <v>309</v>
       </c>
       <c r="Q49" s="56" t="s">
         <v>77</v>
@@ -7591,7 +7560,7 @@
       <c r="S49" s="60"/>
       <c r="T49" s="150"/>
       <c r="U49" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V49" s="180"/>
       <c r="W49" s="61"/>
@@ -7608,19 +7577,19 @@
     </row>
     <row r="50" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A50" s="39" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="B50" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C50" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D50" s="29" t="s">
         <v>285</v>
       </c>
       <c r="E50" s="55" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="F50" s="54" t="s">
         <v>77</v>
@@ -7629,7 +7598,7 @@
         <v>93</v>
       </c>
       <c r="H50" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I50" s="20" t="s">
         <v>102</v>
@@ -7645,7 +7614,7 @@
       <c r="N50" s="57"/>
       <c r="O50" s="149"/>
       <c r="P50" s="30" t="s">
-        <v>333</v>
+        <v>308</v>
       </c>
       <c r="Q50" s="56" t="s">
         <v>77</v>
@@ -7654,7 +7623,7 @@
       <c r="S50" s="60"/>
       <c r="T50" s="150"/>
       <c r="U50" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V50" s="180"/>
       <c r="W50" s="61"/>
@@ -7671,19 +7640,19 @@
     </row>
     <row r="51" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A51" s="39" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="B51" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C51" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D51" s="29" t="s">
         <v>285</v>
       </c>
       <c r="E51" s="55" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="F51" s="54" t="s">
         <v>77</v>
@@ -7692,7 +7661,7 @@
         <v>93</v>
       </c>
       <c r="H51" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I51" s="20" t="s">
         <v>102</v>
@@ -7707,8 +7676,8 @@
       <c r="M51" s="58"/>
       <c r="N51" s="57"/>
       <c r="O51" s="149"/>
-      <c r="P51" s="30" t="s">
-        <v>325</v>
+      <c r="P51" s="166" t="s">
+        <v>314</v>
       </c>
       <c r="Q51" s="56" t="s">
         <v>77</v>
@@ -7717,7 +7686,7 @@
       <c r="S51" s="60"/>
       <c r="T51" s="150"/>
       <c r="U51" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V51" s="180"/>
       <c r="W51" s="61"/>
@@ -7734,19 +7703,19 @@
     </row>
     <row r="52" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A52" s="39" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="B52" s="53" t="s">
         <v>37</v>
       </c>
       <c r="C52" s="54" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="D52" s="29" t="s">
         <v>285</v>
       </c>
       <c r="E52" s="55" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="F52" s="54" t="s">
         <v>77</v>
@@ -7755,7 +7724,7 @@
         <v>93</v>
       </c>
       <c r="H52" s="210" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="I52" s="20" t="s">
         <v>102</v>
@@ -7770,8 +7739,8 @@
       <c r="M52" s="58"/>
       <c r="N52" s="57"/>
       <c r="O52" s="149"/>
-      <c r="P52" s="30" t="s">
-        <v>326</v>
+      <c r="P52" s="190" t="s">
+        <v>324</v>
       </c>
       <c r="Q52" s="56" t="s">
         <v>77</v>
@@ -7780,7 +7749,7 @@
       <c r="S52" s="60"/>
       <c r="T52" s="150"/>
       <c r="U52" s="21" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="V52" s="180"/>
       <c r="W52" s="61"/>
@@ -7796,60 +7765,30 @@
       <c r="AE52" s="58"/>
     </row>
     <row r="53" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
-      <c r="A53" s="39" t="s">
-        <v>477</v>
-      </c>
-      <c r="B53" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C53" s="54" t="s">
-        <v>354</v>
-      </c>
-      <c r="D53" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E53" s="55" t="s">
-        <v>473</v>
-      </c>
-      <c r="F53" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="G53" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="H53" s="210" t="s">
-        <v>357</v>
-      </c>
-      <c r="I53" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J53" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="K53" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A53" s="39"/>
+      <c r="B53" s="53"/>
+      <c r="C53" s="54"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="54"/>
+      <c r="G53" s="56"/>
+      <c r="H53" s="210"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="53"/>
+      <c r="K53" s="28"/>
       <c r="L53" s="149"/>
       <c r="M53" s="58"/>
       <c r="N53" s="57"/>
       <c r="O53" s="149"/>
-      <c r="P53" s="30" t="s">
-        <v>337</v>
-      </c>
-      <c r="Q53" s="56" t="s">
-        <v>77</v>
-      </c>
+      <c r="P53" s="30"/>
+      <c r="Q53" s="56"/>
       <c r="R53" s="59"/>
       <c r="S53" s="60"/>
       <c r="T53" s="150"/>
-      <c r="U53" s="21" t="s">
-        <v>486</v>
-      </c>
+      <c r="U53" s="21"/>
       <c r="V53" s="180"/>
       <c r="W53" s="61"/>
-      <c r="X53" s="21">
-        <v>100</v>
-      </c>
+      <c r="X53" s="21"/>
       <c r="Y53" s="151"/>
       <c r="Z53" s="62"/>
       <c r="AA53" s="62"/>
@@ -7859,60 +7798,30 @@
       <c r="AE53" s="58"/>
     </row>
     <row r="54" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
-      <c r="A54" s="39" t="s">
-        <v>478</v>
-      </c>
-      <c r="B54" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C54" s="54" t="s">
-        <v>354</v>
-      </c>
-      <c r="D54" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E54" s="55" t="s">
-        <v>473</v>
-      </c>
-      <c r="F54" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="G54" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="H54" s="210" t="s">
-        <v>357</v>
-      </c>
-      <c r="I54" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J54" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="K54" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A54" s="39"/>
+      <c r="B54" s="53"/>
+      <c r="C54" s="54"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="55"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="56"/>
+      <c r="H54" s="210"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="53"/>
+      <c r="K54" s="28"/>
       <c r="L54" s="149"/>
       <c r="M54" s="58"/>
       <c r="N54" s="57"/>
       <c r="O54" s="149"/>
-      <c r="P54" s="30" t="s">
-        <v>314</v>
-      </c>
-      <c r="Q54" s="56" t="s">
-        <v>77</v>
-      </c>
+      <c r="P54" s="30"/>
+      <c r="Q54" s="56"/>
       <c r="R54" s="59"/>
       <c r="S54" s="60"/>
       <c r="T54" s="150"/>
-      <c r="U54" s="21" t="s">
-        <v>486</v>
-      </c>
+      <c r="U54" s="21"/>
       <c r="V54" s="180"/>
       <c r="W54" s="61"/>
-      <c r="X54" s="21">
-        <v>100</v>
-      </c>
+      <c r="X54" s="21"/>
       <c r="Y54" s="151"/>
       <c r="Z54" s="62"/>
       <c r="AA54" s="62"/>
@@ -7922,60 +7831,30 @@
       <c r="AE54" s="58"/>
     </row>
     <row r="55" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
-      <c r="A55" s="39" t="s">
-        <v>479</v>
-      </c>
-      <c r="B55" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C55" s="54" t="s">
-        <v>354</v>
-      </c>
-      <c r="D55" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E55" s="55" t="s">
-        <v>473</v>
-      </c>
-      <c r="F55" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="G55" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="H55" s="210" t="s">
-        <v>357</v>
-      </c>
-      <c r="I55" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J55" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="K55" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A55" s="39"/>
+      <c r="B55" s="53"/>
+      <c r="C55" s="54"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="54"/>
+      <c r="G55" s="56"/>
+      <c r="H55" s="210"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="53"/>
+      <c r="K55" s="28"/>
       <c r="L55" s="149"/>
       <c r="M55" s="58"/>
       <c r="N55" s="57"/>
       <c r="O55" s="149"/>
-      <c r="P55" s="30" t="s">
-        <v>313</v>
-      </c>
-      <c r="Q55" s="56" t="s">
-        <v>77</v>
-      </c>
+      <c r="P55" s="30"/>
+      <c r="Q55" s="56"/>
       <c r="R55" s="59"/>
       <c r="S55" s="60"/>
       <c r="T55" s="150"/>
-      <c r="U55" s="21" t="s">
-        <v>486</v>
-      </c>
+      <c r="U55" s="21"/>
       <c r="V55" s="180"/>
       <c r="W55" s="61"/>
-      <c r="X55" s="21">
-        <v>100</v>
-      </c>
+      <c r="X55" s="21"/>
       <c r="Y55" s="151"/>
       <c r="Z55" s="62"/>
       <c r="AA55" s="62"/>
@@ -7985,60 +7864,30 @@
       <c r="AE55" s="58"/>
     </row>
     <row r="56" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
-      <c r="A56" s="39" t="s">
-        <v>480</v>
-      </c>
-      <c r="B56" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C56" s="54" t="s">
-        <v>354</v>
-      </c>
-      <c r="D56" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E56" s="55" t="s">
-        <v>473</v>
-      </c>
-      <c r="F56" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="G56" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="H56" s="210" t="s">
-        <v>357</v>
-      </c>
-      <c r="I56" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J56" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="K56" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A56" s="39"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="55"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="56"/>
+      <c r="H56" s="210"/>
+      <c r="I56" s="20"/>
+      <c r="J56" s="53"/>
+      <c r="K56" s="28"/>
       <c r="L56" s="149"/>
       <c r="M56" s="58"/>
       <c r="N56" s="57"/>
       <c r="O56" s="149"/>
-      <c r="P56" s="166" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q56" s="56" t="s">
-        <v>77</v>
-      </c>
+      <c r="P56" s="166"/>
+      <c r="Q56" s="56"/>
       <c r="R56" s="59"/>
       <c r="S56" s="60"/>
       <c r="T56" s="150"/>
-      <c r="U56" s="21" t="s">
-        <v>486</v>
-      </c>
+      <c r="U56" s="21"/>
       <c r="V56" s="180"/>
       <c r="W56" s="61"/>
-      <c r="X56" s="21">
-        <v>100</v>
-      </c>
+      <c r="X56" s="21"/>
       <c r="Y56" s="151"/>
       <c r="Z56" s="62"/>
       <c r="AA56" s="62"/>
@@ -8048,60 +7897,30 @@
       <c r="AE56" s="58"/>
     </row>
     <row r="57" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
-      <c r="A57" s="39" t="s">
-        <v>481</v>
-      </c>
-      <c r="B57" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C57" s="54" t="s">
-        <v>354</v>
-      </c>
-      <c r="D57" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E57" s="55" t="s">
-        <v>473</v>
-      </c>
-      <c r="F57" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="G57" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="H57" s="210" t="s">
-        <v>357</v>
-      </c>
-      <c r="I57" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J57" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="K57" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A57" s="39"/>
+      <c r="B57" s="53"/>
+      <c r="C57" s="54"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="55"/>
+      <c r="F57" s="54"/>
+      <c r="G57" s="56"/>
+      <c r="H57" s="210"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="53"/>
+      <c r="K57" s="28"/>
       <c r="L57" s="149"/>
       <c r="M57" s="58"/>
       <c r="N57" s="57"/>
       <c r="O57" s="149"/>
-      <c r="P57" s="190" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q57" s="56" t="s">
-        <v>77</v>
-      </c>
+      <c r="P57" s="190"/>
+      <c r="Q57" s="56"/>
       <c r="R57" s="59"/>
       <c r="S57" s="60"/>
       <c r="T57" s="150"/>
-      <c r="U57" s="21" t="s">
-        <v>486</v>
-      </c>
+      <c r="U57" s="21"/>
       <c r="V57" s="180"/>
       <c r="W57" s="61"/>
-      <c r="X57" s="21">
-        <v>100</v>
-      </c>
+      <c r="X57" s="21"/>
       <c r="Y57" s="151"/>
       <c r="Z57" s="62"/>
       <c r="AA57" s="62"/>
@@ -19537,12 +19356,6 @@
           </x14:formula1>
           <xm:sqref>H15:H394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!$M$3:$M$45</xm:f>
-          </x14:formula1>
-          <xm:sqref>P15:P394</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DB8F3B2-ED07-314E-8B12-E986A210F9E2}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$K$3:$K$6</xm:f>
@@ -19554,6 +19367,12 @@
             <xm:f>'Drop down lists'!$C$3:$C$41</xm:f>
           </x14:formula1>
           <xm:sqref>D15:D394</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!$M$3:$M$40</xm:f>
+          </x14:formula1>
+          <xm:sqref>P15:P394</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -19568,8 +19387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AL103"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M45"/>
+    <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -19636,7 +19455,7 @@
         <v>284</v>
       </c>
       <c r="K2" s="26" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="L2" s="27" t="s">
         <v>80</v>
@@ -19648,7 +19467,7 @@
         <v>251</v>
       </c>
       <c r="O2" s="189" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="P2" s="43"/>
       <c r="Q2" s="42"/>
@@ -19679,10 +19498,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>15</v>
@@ -19706,19 +19525,19 @@
         <v>300</v>
       </c>
       <c r="K3" s="173" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="L3" s="167" t="s">
         <v>27</v>
       </c>
       <c r="M3" s="30" t="s">
-        <v>303</v>
+        <v>326</v>
       </c>
       <c r="N3" s="175">
         <v>5</v>
       </c>
       <c r="O3" s="174" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="P3" s="21"/>
       <c r="Q3" s="21"/>
@@ -19760,19 +19579,19 @@
         <v>301</v>
       </c>
       <c r="K4" s="173" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="L4" s="168" t="s">
         <v>28</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>304</v>
+        <v>325</v>
       </c>
       <c r="N4" s="175">
         <v>10</v>
       </c>
       <c r="O4" s="174" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="P4" s="21"/>
       <c r="Q4" s="21"/>
@@ -19808,13 +19627,13 @@
         <v>77</v>
       </c>
       <c r="K5" s="196" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="L5" s="168" t="s">
         <v>29</v>
       </c>
       <c r="M5" s="30" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="N5" s="175">
         <v>15</v>
@@ -19831,7 +19650,7 @@
     <row r="6" spans="1:38">
       <c r="A6" s="31"/>
       <c r="B6" s="37" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C6" s="29" t="s">
         <v>286</v>
@@ -19848,13 +19667,13 @@
         <v>102</v>
       </c>
       <c r="K6" s="173" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="L6" s="167" t="s">
         <v>30</v>
       </c>
       <c r="M6" s="30" t="s">
-        <v>331</v>
+        <v>427</v>
       </c>
       <c r="N6" s="175">
         <v>20</v>
@@ -19883,13 +19702,13 @@
         <v>252</v>
       </c>
       <c r="I7" s="169" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="L7" s="168" t="s">
         <v>31</v>
       </c>
       <c r="M7" s="30" t="s">
-        <v>330</v>
+        <v>304</v>
       </c>
       <c r="N7" s="175">
         <v>25</v>
@@ -19915,7 +19734,7 @@
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="173" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
@@ -19925,7 +19744,7 @@
         <v>32</v>
       </c>
       <c r="M8" s="30" t="s">
-        <v>306</v>
+        <v>333</v>
       </c>
       <c r="N8" s="175">
         <v>30</v>
@@ -19951,7 +19770,7 @@
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="173" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
@@ -19961,7 +19780,7 @@
         <v>33</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="N9" s="175">
         <v>35</v>
@@ -19979,7 +19798,7 @@
       <c r="A10" s="31"/>
       <c r="B10" s="7"/>
       <c r="C10" s="29" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="20" t="s">
@@ -19996,8 +19815,8 @@
       <c r="L10" s="168" t="s">
         <v>34</v>
       </c>
-      <c r="M10" s="30" t="s">
-        <v>307</v>
+      <c r="M10" s="165" t="s">
+        <v>369</v>
       </c>
       <c r="N10" s="175">
         <v>40</v>
@@ -20014,7 +19833,7 @@
     <row r="11" spans="1:38">
       <c r="A11" s="31"/>
       <c r="C11" s="29" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="20" t="s">
@@ -20032,7 +19851,7 @@
         <v>105</v>
       </c>
       <c r="M11" s="30" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="N11" s="175">
         <v>45</v>
@@ -20050,7 +19869,7 @@
       <c r="A12" s="31"/>
       <c r="B12" s="32"/>
       <c r="C12" s="29" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="20" t="s">
@@ -20068,7 +19887,7 @@
         <v>106</v>
       </c>
       <c r="M12" s="30" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="N12" s="175">
         <v>50</v>
@@ -20086,7 +19905,7 @@
       <c r="A13" s="31"/>
       <c r="B13" s="32"/>
       <c r="C13" s="29" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="20" t="s">
@@ -20094,7 +19913,7 @@
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="169" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
@@ -20104,7 +19923,7 @@
         <v>114</v>
       </c>
       <c r="M13" s="30" t="s">
-        <v>339</v>
+        <v>318</v>
       </c>
       <c r="N13" s="175">
         <v>55</v>
@@ -20122,7 +19941,7 @@
       <c r="A14" s="31"/>
       <c r="B14" s="32"/>
       <c r="C14" s="29" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="20" t="s">
@@ -20130,7 +19949,7 @@
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="169" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
@@ -20140,7 +19959,7 @@
         <v>115</v>
       </c>
       <c r="M14" s="30" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="N14" s="175">
         <v>60</v>
@@ -20158,7 +19977,7 @@
       <c r="A15" s="31"/>
       <c r="B15" s="32"/>
       <c r="C15" s="29" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="20" t="s">
@@ -20175,8 +19994,8 @@
       <c r="L15" s="168" t="s">
         <v>116</v>
       </c>
-      <c r="M15" s="165" t="s">
-        <v>375</v>
+      <c r="M15" s="30" t="s">
+        <v>307</v>
       </c>
       <c r="N15" s="175">
         <v>65</v>
@@ -20194,7 +20013,7 @@
       <c r="A16" s="31"/>
       <c r="B16" s="33"/>
       <c r="C16" s="29" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="20" t="s">
@@ -20208,8 +20027,8 @@
       <c r="L16" s="168" t="s">
         <v>117</v>
       </c>
-      <c r="M16" s="30" t="s">
-        <v>310</v>
+      <c r="M16" s="165" t="s">
+        <v>367</v>
       </c>
       <c r="N16" s="175">
         <v>70</v>
@@ -20227,7 +20046,7 @@
       <c r="A17" s="31"/>
       <c r="B17" s="33"/>
       <c r="C17" s="29" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="20" t="s">
@@ -20243,7 +20062,7 @@
         <v>118</v>
       </c>
       <c r="M17" s="30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="N17" s="175">
         <v>75</v>
@@ -20261,7 +20080,7 @@
       <c r="A18" s="31"/>
       <c r="B18" s="33"/>
       <c r="C18" s="29" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="20" t="s">
@@ -20277,7 +20096,7 @@
         <v>119</v>
       </c>
       <c r="M18" s="30" t="s">
-        <v>323</v>
+        <v>365</v>
       </c>
       <c r="N18" s="175">
         <v>80</v>
@@ -20295,7 +20114,7 @@
       <c r="A19" s="31"/>
       <c r="B19" s="33"/>
       <c r="C19" s="29" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="20" t="s">
@@ -20311,7 +20130,7 @@
         <v>107</v>
       </c>
       <c r="M19" s="30" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="N19" s="175">
         <v>85</v>
@@ -20329,7 +20148,7 @@
       <c r="A20" s="31"/>
       <c r="B20" s="33"/>
       <c r="C20" s="29" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="20" t="s">
@@ -20345,7 +20164,7 @@
         <v>129</v>
       </c>
       <c r="M20" s="30" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="N20" s="175">
         <v>90</v>
@@ -20363,7 +20182,7 @@
       <c r="A21" s="31"/>
       <c r="B21" s="33"/>
       <c r="C21" s="29" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="20" t="s">
@@ -20378,8 +20197,8 @@
       <c r="L21" s="168" t="s">
         <v>108</v>
       </c>
-      <c r="M21" s="165" t="s">
-        <v>373</v>
+      <c r="M21" s="30" t="s">
+        <v>315</v>
       </c>
       <c r="N21" s="175">
         <v>95</v>
@@ -20397,7 +20216,7 @@
       <c r="A22" s="31"/>
       <c r="B22" s="33"/>
       <c r="C22" s="29" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="20" t="s">
@@ -20412,8 +20231,8 @@
       <c r="L22" s="167" t="s">
         <v>109</v>
       </c>
-      <c r="M22" s="30" t="s">
-        <v>315</v>
+      <c r="M22" s="165" t="s">
+        <v>368</v>
       </c>
       <c r="N22" s="175">
         <v>100</v>
@@ -20431,7 +20250,7 @@
       <c r="A23" s="31"/>
       <c r="B23" s="33"/>
       <c r="C23" s="29" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="20" t="s">
@@ -20447,7 +20266,7 @@
         <v>110</v>
       </c>
       <c r="M23" s="30" t="s">
-        <v>371</v>
+        <v>330</v>
       </c>
       <c r="O23" s="21"/>
       <c r="P23" s="21"/>
@@ -20462,7 +20281,7 @@
       <c r="A24" s="31"/>
       <c r="B24" s="33"/>
       <c r="C24" s="29" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="20" t="s">
@@ -20478,7 +20297,7 @@
         <v>111</v>
       </c>
       <c r="M24" s="30" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="O24" s="21"/>
       <c r="P24" s="21"/>
@@ -20493,7 +20312,7 @@
       <c r="A25" s="31"/>
       <c r="B25" s="33"/>
       <c r="C25" s="29" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="20" t="s">
@@ -20509,7 +20328,7 @@
         <v>112</v>
       </c>
       <c r="M25" s="30" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="O25" s="21"/>
       <c r="P25" s="21"/>
@@ -20524,7 +20343,7 @@
       <c r="A26" s="31"/>
       <c r="B26" s="33"/>
       <c r="C26" s="29" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="20" t="s">
@@ -20539,8 +20358,8 @@
       <c r="L26" s="168" t="s">
         <v>113</v>
       </c>
-      <c r="M26" s="30" t="s">
-        <v>320</v>
+      <c r="M26" s="165" t="s">
+        <v>366</v>
       </c>
       <c r="O26" s="21"/>
       <c r="P26" s="21"/>
@@ -20555,7 +20374,7 @@
       <c r="A27" s="31"/>
       <c r="B27" s="33"/>
       <c r="C27" s="29" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="D27" s="21"/>
       <c r="E27" s="20" t="s">
@@ -20570,8 +20389,8 @@
       <c r="L27" s="167" t="s">
         <v>120</v>
       </c>
-      <c r="M27" s="165" t="s">
-        <v>374</v>
+      <c r="M27" s="30" t="s">
+        <v>319</v>
       </c>
       <c r="O27" s="21"/>
       <c r="P27" s="21"/>
@@ -20602,7 +20421,7 @@
         <v>130</v>
       </c>
       <c r="M28" s="30" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="O28" s="21"/>
       <c r="P28" s="21"/>
@@ -20617,7 +20436,7 @@
       <c r="A29" s="31"/>
       <c r="B29" s="33"/>
       <c r="C29" s="29" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="20" t="s">
@@ -20633,7 +20452,7 @@
         <v>139</v>
       </c>
       <c r="M29" s="30" t="s">
-        <v>340</v>
+        <v>311</v>
       </c>
       <c r="O29" s="21"/>
       <c r="P29" s="21"/>
@@ -20648,7 +20467,7 @@
       <c r="A30" s="31"/>
       <c r="B30" s="33"/>
       <c r="C30" s="29" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="20" t="s">
@@ -20664,7 +20483,7 @@
         <v>148</v>
       </c>
       <c r="M30" s="30" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="O30" s="21"/>
       <c r="P30" s="21"/>
@@ -20679,7 +20498,7 @@
       <c r="A31" s="21"/>
       <c r="B31" s="33"/>
       <c r="C31" s="29" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="20" t="s">
@@ -20694,8 +20513,8 @@
       <c r="L31" s="168" t="s">
         <v>157</v>
       </c>
-      <c r="M31" s="165" t="s">
-        <v>372</v>
+      <c r="M31" s="30" t="s">
+        <v>313</v>
       </c>
       <c r="O31" s="21"/>
       <c r="P31" s="21"/>
@@ -20710,7 +20529,7 @@
       <c r="A32" s="21"/>
       <c r="B32" s="33"/>
       <c r="C32" s="29" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="20" t="s">
@@ -20726,7 +20545,7 @@
         <v>166</v>
       </c>
       <c r="M32" s="30" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="O32" s="21"/>
       <c r="P32" s="21"/>
@@ -20741,7 +20560,7 @@
       <c r="A33" s="21"/>
       <c r="B33" s="33"/>
       <c r="C33" s="29" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="20" t="s">
@@ -20757,7 +20576,7 @@
         <v>175</v>
       </c>
       <c r="M33" s="30" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="O33" s="21"/>
       <c r="P33" s="21"/>
@@ -20772,7 +20591,7 @@
       <c r="A34" s="21"/>
       <c r="B34" s="33"/>
       <c r="C34" s="29" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="20" t="s">
@@ -20788,7 +20607,7 @@
         <v>184</v>
       </c>
       <c r="M34" s="30" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="O34" s="21"/>
       <c r="P34" s="21"/>
@@ -20803,7 +20622,7 @@
       <c r="A35" s="21"/>
       <c r="B35" s="33"/>
       <c r="C35" s="29" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="20" t="s">
@@ -20819,7 +20638,7 @@
         <v>121</v>
       </c>
       <c r="M35" s="30" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="O35" s="21"/>
       <c r="P35" s="21"/>
@@ -20834,7 +20653,7 @@
       <c r="A36" s="21"/>
       <c r="B36" s="33"/>
       <c r="C36" s="29" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="20" t="s">
@@ -20850,7 +20669,7 @@
         <v>131</v>
       </c>
       <c r="M36" s="30" t="s">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="O36" s="21"/>
       <c r="P36" s="21"/>
@@ -20865,7 +20684,7 @@
       <c r="A37" s="21"/>
       <c r="B37" s="33"/>
       <c r="C37" s="29" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="20" t="s">
@@ -20881,7 +20700,7 @@
         <v>140</v>
       </c>
       <c r="M37" s="30" t="s">
-        <v>335</v>
+        <v>309</v>
       </c>
       <c r="O37" s="21"/>
       <c r="P37" s="21"/>
@@ -20896,7 +20715,7 @@
       <c r="A38" s="21"/>
       <c r="B38" s="33"/>
       <c r="C38" s="29" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="20" t="s">
@@ -20912,7 +20731,7 @@
         <v>149</v>
       </c>
       <c r="M38" s="30" t="s">
-        <v>333</v>
+        <v>308</v>
       </c>
       <c r="O38" s="21"/>
       <c r="P38" s="21"/>
@@ -20927,7 +20746,7 @@
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="29" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="20" t="s">
@@ -20942,8 +20761,8 @@
       <c r="L39" s="168" t="s">
         <v>158</v>
       </c>
-      <c r="M39" s="30" t="s">
-        <v>325</v>
+      <c r="M39" s="166" t="s">
+        <v>314</v>
       </c>
       <c r="O39" s="21"/>
       <c r="P39" s="21"/>
@@ -20958,7 +20777,7 @@
       <c r="A40" s="21"/>
       <c r="B40" s="21"/>
       <c r="C40" s="29" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="20" t="s">
@@ -20973,8 +20792,8 @@
       <c r="L40" s="168" t="s">
         <v>167</v>
       </c>
-      <c r="M40" s="30" t="s">
-        <v>326</v>
+      <c r="M40" s="190" t="s">
+        <v>324</v>
       </c>
       <c r="O40" s="21"/>
       <c r="P40" s="21"/>
@@ -20989,7 +20808,7 @@
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
       <c r="C41" s="29" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="D41" s="21"/>
       <c r="E41" s="20" t="s">
@@ -21004,9 +20823,6 @@
       <c r="L41" s="167" t="s">
         <v>176</v>
       </c>
-      <c r="M41" s="30" t="s">
-        <v>337</v>
-      </c>
       <c r="O41" s="21"/>
       <c r="P41" s="21"/>
       <c r="Q41" s="21"/>
@@ -21033,9 +20849,6 @@
       <c r="L42" s="168" t="s">
         <v>185</v>
       </c>
-      <c r="M42" s="30" t="s">
-        <v>314</v>
-      </c>
       <c r="O42" s="21"/>
       <c r="P42" s="21"/>
       <c r="Q42" s="21"/>
@@ -21062,9 +20875,6 @@
       <c r="L43" s="167" t="s">
         <v>122</v>
       </c>
-      <c r="M43" s="30" t="s">
-        <v>313</v>
-      </c>
       <c r="O43" s="21"/>
       <c r="P43" s="21"/>
       <c r="Q43" s="21"/>
@@ -21091,9 +20901,6 @@
       <c r="L44" s="168" t="s">
         <v>132</v>
       </c>
-      <c r="M44" s="166" t="s">
-        <v>319</v>
-      </c>
       <c r="O44" s="21"/>
       <c r="P44" s="21"/>
       <c r="Q44" s="21"/>
@@ -21119,9 +20926,6 @@
       <c r="K45" s="21"/>
       <c r="L45" s="168" t="s">
         <v>141</v>
-      </c>
-      <c r="M45" s="190" t="s">
-        <v>329</v>
       </c>
       <c r="O45" s="21"/>
       <c r="P45" s="21"/>
@@ -22610,7 +22414,7 @@
       <c r="V103" s="21"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="OJFtPcw1Smz57zpSg0eibTEQTykzI9svcg7GftP2lBA7QFS7NCmOzJsoXM5Eo+ed1/q0N92EfhKxmpnlEtGw+Q==" saltValue="k9ec4vayQ7/FAqum2SCTzA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="uxJy/XrZi++fwQPYouH/a3p2Wm6PiJRc24f/QvFMm7ET2neUcru3FQ49VUn/O81LUvV0hDW7Y3nePwBP5GGaBQ==" saltValue="eogzL5c1zcehI3Rfw/sv6w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>